<commit_message>
add new sheet of SBT
</commit_message>
<xml_diff>
--- a/JavaExcelBDD/src/test/resources/ExcelBDD.xlsx
+++ b/JavaExcelBDD/src/test/resources/ExcelBDD.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mike\git\CodeKata\CodeKata-core\src\test\java\kata\excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/2fe8b90741a02718/Git/SimpleOpenExcelBDD/JavaExcelBDD/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A430A62-E059-4E93-9246-F6CA9FBCEE71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{79812025-A047-44C4-86A7-E2AEC82C8710}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="6" xr2:uid="{965C72BA-AC7B-4020-96A1-B4855C2F0853}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="7" xr2:uid="{965C72BA-AC7B-4020-96A1-B4855C2F0853}"/>
   </bookViews>
   <sheets>
     <sheet name="SimpleOpenBDD" sheetId="1" r:id="rId1"/>
@@ -18,10 +18,11 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId3"/>
     <sheet name="Sheet3" sheetId="4" r:id="rId4"/>
     <sheet name="Sheet4" sheetId="6" r:id="rId5"/>
-    <sheet name="Sheet5" sheetId="7" r:id="rId6"/>
-    <sheet name="StoryExample1" sheetId="8" r:id="rId7"/>
+    <sheet name="StoryExample1" sheetId="8" r:id="rId6"/>
+    <sheet name="SBT" sheetId="9" r:id="rId7"/>
+    <sheet name="SBTSheet1" sheetId="7" r:id="rId8"/>
   </sheets>
-  <calcPr calcId="191029" concurrentCalc="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="384" uniqueCount="163">
   <si>
     <t>Role</t>
   </si>
@@ -464,6 +465,72 @@
   </si>
   <si>
     <t>NanJing</t>
+  </si>
+  <si>
+    <t>SBTSheet1</t>
+  </si>
+  <si>
+    <t>Input</t>
+  </si>
+  <si>
+    <t>Expected</t>
+  </si>
+  <si>
+    <t>Test Result</t>
+  </si>
+  <si>
+    <t>pass</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Header</t>
+  </si>
+  <si>
+    <t>Sub-Step</t>
+  </si>
+  <si>
+    <t>ExcelFileName</t>
+  </si>
+  <si>
+    <t>Dev</t>
+  </si>
+  <si>
+    <t>select file</t>
+  </si>
+  <si>
+    <t>select sheet</t>
+  </si>
+  <si>
+    <t>Get data from Excel</t>
+  </si>
+  <si>
+    <t>Get first Input</t>
+  </si>
+  <si>
+    <t>Get first Expected</t>
+  </si>
+  <si>
+    <t>Get first test result</t>
+  </si>
+  <si>
+    <t>check error</t>
+  </si>
+  <si>
+    <t>FirstInput</t>
+  </si>
+  <si>
+    <t>FirstExpected</t>
+  </si>
+  <si>
+    <t>FirstTestResult</t>
+  </si>
+  <si>
+    <t>failed</t>
+  </si>
+  <si>
+    <t>FailedWord</t>
+  </si>
+  <si>
+    <t>StepID</t>
   </si>
 </sst>
 </file>
@@ -536,7 +603,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -575,6 +642,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -753,7 +832,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="82">
+  <cellXfs count="93">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -831,6 +910,14 @@
     <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -965,6 +1052,27 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1383,7 +1491,7 @@
   <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K12" sqref="K12"/>
+      <selection sqref="A1:E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1669,66 +1777,66 @@
       <c r="H11" s="7"/>
     </row>
     <row r="12" spans="1:8" ht="45">
-      <c r="A12" s="40">
+      <c r="A12" s="44">
         <v>11</v>
       </c>
       <c r="B12" s="24" t="s">
         <v>89</v>
       </c>
-      <c r="C12" s="43" t="s">
+      <c r="C12" s="47" t="s">
         <v>5</v>
       </c>
-      <c r="D12" s="44" t="s">
+      <c r="D12" s="48" t="s">
         <v>86</v>
       </c>
-      <c r="E12" s="37">
+      <c r="E12" s="41">
         <v>3</v>
       </c>
-      <c r="F12" s="37">
+      <c r="F12" s="41">
         <v>3</v>
       </c>
-      <c r="G12" s="37">
+      <c r="G12" s="41">
         <v>3</v>
       </c>
-      <c r="H12" s="37">
+      <c r="H12" s="41">
         <v>3</v>
       </c>
     </row>
     <row r="13" spans="1:8">
-      <c r="A13" s="41"/>
+      <c r="A13" s="45"/>
       <c r="B13" s="21" t="s">
         <v>97</v>
       </c>
-      <c r="C13" s="43"/>
-      <c r="D13" s="45"/>
-      <c r="E13" s="38"/>
-      <c r="F13" s="38"/>
-      <c r="G13" s="38"/>
-      <c r="H13" s="38"/>
+      <c r="C13" s="47"/>
+      <c r="D13" s="49"/>
+      <c r="E13" s="42"/>
+      <c r="F13" s="42"/>
+      <c r="G13" s="42"/>
+      <c r="H13" s="42"/>
     </row>
     <row r="14" spans="1:8">
-      <c r="A14" s="41"/>
+      <c r="A14" s="45"/>
       <c r="B14" s="21" t="s">
         <v>84</v>
       </c>
-      <c r="C14" s="43"/>
-      <c r="D14" s="45"/>
-      <c r="E14" s="38"/>
-      <c r="F14" s="38"/>
-      <c r="G14" s="38"/>
-      <c r="H14" s="38"/>
+      <c r="C14" s="47"/>
+      <c r="D14" s="49"/>
+      <c r="E14" s="42"/>
+      <c r="F14" s="42"/>
+      <c r="G14" s="42"/>
+      <c r="H14" s="42"/>
     </row>
     <row r="15" spans="1:8">
-      <c r="A15" s="42"/>
+      <c r="A15" s="46"/>
       <c r="B15" s="22" t="s">
         <v>85</v>
       </c>
-      <c r="C15" s="43"/>
-      <c r="D15" s="46"/>
-      <c r="E15" s="39"/>
-      <c r="F15" s="39"/>
-      <c r="G15" s="39"/>
-      <c r="H15" s="39"/>
+      <c r="C15" s="47"/>
+      <c r="D15" s="50"/>
+      <c r="E15" s="43"/>
+      <c r="F15" s="43"/>
+      <c r="G15" s="43"/>
+      <c r="H15" s="43"/>
     </row>
     <row r="16" spans="1:8" ht="30">
       <c r="A16" s="26">
@@ -1802,7 +1910,7 @@
   <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="B29" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1910,7 +2018,7 @@
       <c r="G6" s="19"/>
     </row>
     <row r="7" spans="1:7">
-      <c r="A7" s="47" t="s">
+      <c r="A7" s="51" t="s">
         <v>77</v>
       </c>
       <c r="B7" s="4" t="s">
@@ -1923,7 +2031,7 @@
       <c r="G7" s="19"/>
     </row>
     <row r="8" spans="1:7">
-      <c r="A8" s="48"/>
+      <c r="A8" s="52"/>
       <c r="B8" s="4" t="s">
         <v>83</v>
       </c>
@@ -1934,7 +2042,7 @@
       <c r="G8" s="19"/>
     </row>
     <row r="9" spans="1:7">
-      <c r="A9" s="49" t="s">
+      <c r="A9" s="53" t="s">
         <v>78</v>
       </c>
       <c r="B9" s="4" t="s">
@@ -1957,7 +2065,7 @@
       </c>
     </row>
     <row r="10" spans="1:7">
-      <c r="A10" s="50"/>
+      <c r="A10" s="54"/>
       <c r="B10" s="15" t="s">
         <v>83</v>
       </c>
@@ -2229,15 +2337,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="51" t="s">
+      <c r="A1" s="55" t="s">
         <v>43</v>
       </c>
-      <c r="B1" s="51"/>
-      <c r="C1" s="51"/>
-      <c r="D1" s="51"/>
-      <c r="E1" s="51"/>
-      <c r="F1" s="51"/>
-      <c r="G1" s="51"/>
+      <c r="B1" s="55"/>
+      <c r="C1" s="55"/>
+      <c r="D1" s="55"/>
+      <c r="E1" s="55"/>
+      <c r="F1" s="55"/>
+      <c r="G1" s="55"/>
       <c r="H1" s="2"/>
     </row>
     <row r="2" spans="1:8">
@@ -2273,7 +2381,7 @@
       <c r="B3" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="C3" s="52" t="s">
+      <c r="C3" s="56" t="s">
         <v>46</v>
       </c>
       <c r="D3" s="4" t="s">
@@ -2299,7 +2407,7 @@
       <c r="B4" s="9" t="s">
         <v>76</v>
       </c>
-      <c r="C4" s="53"/>
+      <c r="C4" s="57"/>
       <c r="D4" s="4" t="s">
         <v>14</v>
       </c>
@@ -2323,7 +2431,7 @@
       <c r="B5" s="9" t="s">
         <v>77</v>
       </c>
-      <c r="C5" s="54"/>
+      <c r="C5" s="58"/>
       <c r="D5" s="4" t="s">
         <v>15</v>
       </c>
@@ -2401,42 +2509,42 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
-      <c r="A1" s="57" t="s">
+      <c r="A1" s="61" t="s">
         <v>50</v>
       </c>
-      <c r="B1" s="57"/>
-      <c r="C1" s="51" t="s">
+      <c r="B1" s="61"/>
+      <c r="C1" s="55" t="s">
         <v>64</v>
       </c>
-      <c r="D1" s="51"/>
+      <c r="D1" s="55"/>
       <c r="E1" s="14" t="s">
         <v>51</v>
       </c>
-      <c r="F1" s="55" t="s">
+      <c r="F1" s="59" t="s">
         <v>52</v>
       </c>
-      <c r="G1" s="56"/>
-      <c r="H1" s="56"/>
-      <c r="I1" s="56"/>
+      <c r="G1" s="60"/>
+      <c r="H1" s="60"/>
+      <c r="I1" s="60"/>
     </row>
     <row r="2" spans="1:9">
-      <c r="A2" s="57" t="s">
+      <c r="A2" s="61" t="s">
         <v>53</v>
       </c>
-      <c r="B2" s="57"/>
-      <c r="C2" s="63" t="s">
+      <c r="B2" s="61"/>
+      <c r="C2" s="67" t="s">
         <v>49</v>
       </c>
-      <c r="D2" s="63"/>
+      <c r="D2" s="67"/>
       <c r="E2" s="11" t="s">
         <v>80</v>
       </c>
-      <c r="F2" s="61" t="s">
+      <c r="F2" s="65" t="s">
         <v>81</v>
       </c>
-      <c r="G2" s="61"/>
-      <c r="H2" s="61"/>
-      <c r="I2" s="62"/>
+      <c r="G2" s="65"/>
+      <c r="H2" s="65"/>
+      <c r="I2" s="66"/>
     </row>
     <row r="3" spans="1:9">
       <c r="A3" s="13" t="s">
@@ -2468,16 +2576,16 @@
       </c>
     </row>
     <row r="4" spans="1:9" ht="69.95" customHeight="1">
-      <c r="A4" s="58" t="s">
+      <c r="A4" s="62" t="s">
         <v>57</v>
       </c>
       <c r="B4" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="C4" s="58" t="s">
+      <c r="C4" s="62" t="s">
         <v>48</v>
       </c>
-      <c r="D4" s="52" t="s">
+      <c r="D4" s="56" t="s">
         <v>46</v>
       </c>
       <c r="E4" s="4" t="s">
@@ -2497,12 +2605,12 @@
       </c>
     </row>
     <row r="5" spans="1:9" ht="69.95" customHeight="1">
-      <c r="A5" s="59"/>
+      <c r="A5" s="63"/>
       <c r="B5" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="C5" s="59"/>
-      <c r="D5" s="53"/>
+      <c r="C5" s="63"/>
+      <c r="D5" s="57"/>
       <c r="E5" s="4" t="s">
         <v>14</v>
       </c>
@@ -2520,12 +2628,12 @@
       </c>
     </row>
     <row r="6" spans="1:9" ht="69.95" customHeight="1">
-      <c r="A6" s="59"/>
+      <c r="A6" s="63"/>
       <c r="B6" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="C6" s="60"/>
-      <c r="D6" s="54"/>
+      <c r="C6" s="64"/>
+      <c r="D6" s="58"/>
       <c r="E6" s="4" t="s">
         <v>15</v>
       </c>
@@ -2535,7 +2643,7 @@
       <c r="I6" s="8"/>
     </row>
     <row r="7" spans="1:9">
-      <c r="A7" s="60"/>
+      <c r="A7" s="64"/>
       <c r="B7" s="9" t="s">
         <v>61</v>
       </c>
@@ -2599,22 +2707,10 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{129A480F-2285-4A8E-88CD-74850D6AFE43}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5B5B253-4765-4799-B65C-A6D3EFCA81AD}">
   <dimension ref="A1:K10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
@@ -2631,41 +2727,41 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="23.25">
-      <c r="A1" s="57" t="s">
+      <c r="A1" s="61" t="s">
         <v>50</v>
       </c>
-      <c r="B1" s="57"/>
-      <c r="C1" s="76" t="s">
+      <c r="B1" s="61"/>
+      <c r="C1" s="80" t="s">
         <v>101</v>
       </c>
-      <c r="D1" s="76"/>
-      <c r="E1" s="76"/>
-      <c r="F1" s="76"/>
-      <c r="G1" s="76"/>
-      <c r="H1" s="76"/>
+      <c r="D1" s="80"/>
+      <c r="E1" s="80"/>
+      <c r="F1" s="80"/>
+      <c r="G1" s="80"/>
+      <c r="H1" s="80"/>
     </row>
     <row r="2" spans="1:11" ht="38.25" customHeight="1">
-      <c r="A2" s="81" t="s">
+      <c r="A2" s="85" t="s">
         <v>53</v>
       </c>
-      <c r="B2" s="81"/>
-      <c r="C2" s="77" t="s">
+      <c r="B2" s="85"/>
+      <c r="C2" s="81" t="s">
         <v>102</v>
       </c>
-      <c r="D2" s="77"/>
-      <c r="E2" s="77"/>
-      <c r="F2" s="77"/>
-      <c r="G2" s="77"/>
-      <c r="H2" s="77"/>
+      <c r="D2" s="81"/>
+      <c r="E2" s="81"/>
+      <c r="F2" s="81"/>
+      <c r="G2" s="81"/>
+      <c r="H2" s="81"/>
     </row>
     <row r="3" spans="1:11">
       <c r="A3" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="78" t="s">
+      <c r="B3" s="82" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="79"/>
+      <c r="C3" s="83"/>
       <c r="D3" s="13" t="s">
         <v>111</v>
       </c>
@@ -2692,14 +2788,14 @@
       </c>
     </row>
     <row r="4" spans="1:11" ht="15" customHeight="1">
-      <c r="A4" s="58" t="s">
+      <c r="A4" s="62" t="s">
         <v>57</v>
       </c>
-      <c r="B4" s="70" t="s">
+      <c r="B4" s="74" t="s">
         <v>104</v>
       </c>
-      <c r="C4" s="71"/>
-      <c r="D4" s="72"/>
+      <c r="C4" s="75"/>
+      <c r="D4" s="76"/>
       <c r="E4" s="31" t="s">
         <v>103</v>
       </c>
@@ -2723,11 +2819,11 @@
       </c>
     </row>
     <row r="5" spans="1:11" ht="51.75" customHeight="1">
-      <c r="A5" s="59"/>
-      <c r="B5" s="80" t="s">
+      <c r="A5" s="63"/>
+      <c r="B5" s="84" t="s">
         <v>107</v>
       </c>
-      <c r="C5" s="80"/>
+      <c r="C5" s="84"/>
       <c r="D5" s="35" t="s">
         <v>113</v>
       </c>
@@ -2754,12 +2850,12 @@
       </c>
     </row>
     <row r="6" spans="1:11" ht="33.75" customHeight="1">
-      <c r="A6" s="59"/>
-      <c r="B6" s="73" t="s">
+      <c r="A6" s="63"/>
+      <c r="B6" s="77" t="s">
         <v>112</v>
       </c>
-      <c r="C6" s="74"/>
-      <c r="D6" s="75"/>
+      <c r="C6" s="78"/>
+      <c r="D6" s="79"/>
       <c r="E6" s="31" t="s">
         <v>109</v>
       </c>
@@ -2783,11 +2879,11 @@
       </c>
     </row>
     <row r="7" spans="1:11" ht="31.5">
-      <c r="A7" s="59"/>
-      <c r="B7" s="64" t="s">
+      <c r="A7" s="63"/>
+      <c r="B7" s="68" t="s">
         <v>110</v>
       </c>
-      <c r="C7" s="65"/>
+      <c r="C7" s="69"/>
       <c r="D7" s="35" t="s">
         <v>114</v>
       </c>
@@ -2814,9 +2910,9 @@
       </c>
     </row>
     <row r="8" spans="1:11" ht="30">
-      <c r="A8" s="59"/>
-      <c r="B8" s="66"/>
-      <c r="C8" s="67"/>
+      <c r="A8" s="63"/>
+      <c r="B8" s="70"/>
+      <c r="C8" s="71"/>
       <c r="D8" s="36" t="s">
         <v>120</v>
       </c>
@@ -2843,9 +2939,9 @@
       </c>
     </row>
     <row r="9" spans="1:11" ht="31.5">
-      <c r="A9" s="59"/>
-      <c r="B9" s="66"/>
-      <c r="C9" s="67"/>
+      <c r="A9" s="63"/>
+      <c r="B9" s="70"/>
+      <c r="C9" s="71"/>
       <c r="D9" s="35" t="s">
         <v>121</v>
       </c>
@@ -2872,9 +2968,9 @@
       </c>
     </row>
     <row r="10" spans="1:11" ht="31.5">
-      <c r="A10" s="60"/>
-      <c r="B10" s="68"/>
-      <c r="C10" s="69"/>
+      <c r="A10" s="64"/>
+      <c r="B10" s="72"/>
+      <c r="C10" s="73"/>
       <c r="D10" s="35" t="s">
         <v>122</v>
       </c>
@@ -2917,4 +3013,506 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACCEE44C-3384-41FF-9A79-FA3C44CB5ED1}">
+  <dimension ref="A4:F13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="21" customWidth="1"/>
+    <col min="2" max="2" width="29" customWidth="1"/>
+    <col min="3" max="3" width="18.28515625" customWidth="1"/>
+    <col min="4" max="4" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="33.85546875" customWidth="1"/>
+    <col min="6" max="6" width="28.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="1:6">
+      <c r="A4" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>147</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="86" t="s">
+        <v>28</v>
+      </c>
+      <c r="B5" s="24" t="s">
+        <v>150</v>
+      </c>
+      <c r="C5" s="26" t="s">
+        <v>149</v>
+      </c>
+      <c r="D5" s="23">
+        <v>1</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>148</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="86"/>
+      <c r="B6" s="24" t="s">
+        <v>151</v>
+      </c>
+      <c r="C6" s="26" t="s">
+        <v>149</v>
+      </c>
+      <c r="D6" s="23">
+        <v>2</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" s="86"/>
+      <c r="B7" s="24" t="s">
+        <v>25</v>
+      </c>
+      <c r="C7" s="26" t="s">
+        <v>149</v>
+      </c>
+      <c r="D7" s="23">
+        <v>3</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="F7" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" s="86"/>
+      <c r="B8" s="24" t="s">
+        <v>27</v>
+      </c>
+      <c r="C8" s="26" t="s">
+        <v>149</v>
+      </c>
+      <c r="D8" s="23">
+        <v>4</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="F8" s="7" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="30">
+      <c r="A9" s="87" t="s">
+        <v>152</v>
+      </c>
+      <c r="B9" s="24" t="s">
+        <v>31</v>
+      </c>
+      <c r="C9" s="26" t="s">
+        <v>5</v>
+      </c>
+      <c r="D9" s="23">
+        <v>5</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="F9" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" s="87"/>
+      <c r="B10" s="24" t="s">
+        <v>153</v>
+      </c>
+      <c r="C10" s="26" t="s">
+        <v>5</v>
+      </c>
+      <c r="D10" s="23">
+        <v>6</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>157</v>
+      </c>
+      <c r="F10" s="7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" s="87"/>
+      <c r="B11" s="24" t="s">
+        <v>154</v>
+      </c>
+      <c r="C11" s="26" t="s">
+        <v>5</v>
+      </c>
+      <c r="D11" s="23">
+        <v>7</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>158</v>
+      </c>
+      <c r="F11" s="7">
+        <v>4.4000000000000004</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" s="87"/>
+      <c r="B12" s="24" t="s">
+        <v>155</v>
+      </c>
+      <c r="C12" s="26" t="s">
+        <v>5</v>
+      </c>
+      <c r="D12" s="23">
+        <v>8</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>159</v>
+      </c>
+      <c r="F12" s="7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" s="87"/>
+      <c r="B13" s="25" t="s">
+        <v>156</v>
+      </c>
+      <c r="C13" s="26" t="s">
+        <v>5</v>
+      </c>
+      <c r="D13" s="23">
+        <v>9</v>
+      </c>
+      <c r="E13" s="6" t="s">
+        <v>161</v>
+      </c>
+      <c r="F13" s="7" t="s">
+        <v>160</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A5:A8"/>
+    <mergeCell ref="A9:A13"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{129A480F-2285-4A8E-88CD-74850D6AFE43}">
+  <dimension ref="A1:N11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="23" customWidth="1"/>
+    <col min="2" max="2" width="25.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.7109375" customWidth="1"/>
+    <col min="5" max="5" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14">
+      <c r="B1" s="38" t="s">
+        <v>146</v>
+      </c>
+      <c r="C1" s="88" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="89"/>
+      <c r="E1" s="90"/>
+      <c r="F1" s="88" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="89"/>
+      <c r="H1" s="90"/>
+      <c r="I1" s="88" t="s">
+        <v>65</v>
+      </c>
+      <c r="J1" s="89"/>
+      <c r="K1" s="90"/>
+      <c r="L1" s="91" t="s">
+        <v>66</v>
+      </c>
+      <c r="M1" s="92"/>
+      <c r="N1" s="92"/>
+    </row>
+    <row r="2" spans="1:14">
+      <c r="A2" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="C2" s="37" t="s">
+        <v>142</v>
+      </c>
+      <c r="D2" s="37" t="s">
+        <v>143</v>
+      </c>
+      <c r="E2" s="37" t="s">
+        <v>144</v>
+      </c>
+      <c r="F2" s="37" t="s">
+        <v>142</v>
+      </c>
+      <c r="G2" s="37" t="s">
+        <v>143</v>
+      </c>
+      <c r="H2" s="37" t="s">
+        <v>144</v>
+      </c>
+      <c r="I2" s="37" t="s">
+        <v>142</v>
+      </c>
+      <c r="J2" s="37" t="s">
+        <v>143</v>
+      </c>
+      <c r="K2" s="37" t="s">
+        <v>144</v>
+      </c>
+      <c r="L2" s="37" t="s">
+        <v>142</v>
+      </c>
+      <c r="M2" s="37" t="s">
+        <v>143</v>
+      </c>
+      <c r="N2" s="37" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14">
+      <c r="A3" s="23" t="s">
+        <v>75</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" s="8" t="str">
+        <f>C3</f>
+        <v>V1.1</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>145</v>
+      </c>
+      <c r="F3" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="G3" s="8" t="str">
+        <f>F3</f>
+        <v>V1.2</v>
+      </c>
+      <c r="H3" s="8" t="s">
+        <v>145</v>
+      </c>
+      <c r="I3" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="J3" s="8" t="str">
+        <f>I3</f>
+        <v>V1.3</v>
+      </c>
+      <c r="K3" s="8" t="s">
+        <v>145</v>
+      </c>
+      <c r="L3" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="M3" s="8" t="str">
+        <f>L3</f>
+        <v>V1.4</v>
+      </c>
+      <c r="N3" s="8" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14">
+      <c r="A4" s="23" t="s">
+        <v>76</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4" s="8" t="str">
+        <f t="shared" ref="D4:D6" si="0">C4</f>
+        <v>V2.1</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>145</v>
+      </c>
+      <c r="F4" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="G4" s="8" t="str">
+        <f t="shared" ref="G4:G6" si="1">F4</f>
+        <v>V2.2</v>
+      </c>
+      <c r="H4" s="8" t="s">
+        <v>145</v>
+      </c>
+      <c r="I4" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="J4" s="8" t="str">
+        <f t="shared" ref="J4:J6" si="2">I4</f>
+        <v>V2.3</v>
+      </c>
+      <c r="K4" s="8" t="s">
+        <v>145</v>
+      </c>
+      <c r="L4" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="M4" s="8" t="str">
+        <f t="shared" ref="M4:M6" si="3">L4</f>
+        <v>V2.4</v>
+      </c>
+      <c r="N4" s="8" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14">
+      <c r="A5" s="39" t="s">
+        <v>77</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="8"/>
+      <c r="D5" s="8"/>
+      <c r="E5" s="8" t="s">
+        <v>145</v>
+      </c>
+      <c r="F5" s="8"/>
+      <c r="G5" s="8"/>
+      <c r="H5" s="8" t="s">
+        <v>145</v>
+      </c>
+      <c r="I5" s="8"/>
+      <c r="J5" s="8"/>
+      <c r="K5" s="8" t="s">
+        <v>145</v>
+      </c>
+      <c r="L5" s="8"/>
+      <c r="M5" s="8"/>
+      <c r="N5" s="8" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14">
+      <c r="A6" s="40" t="s">
+        <v>78</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="30" t="s">
+        <v>100</v>
+      </c>
+      <c r="D6" s="8" t="str">
+        <f t="shared" si="0"/>
+        <v>2021/4/30</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>145</v>
+      </c>
+      <c r="F6" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="G6" s="8" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H6" s="8" t="s">
+        <v>145</v>
+      </c>
+      <c r="I6" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="J6" s="8" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="K6" s="8" t="s">
+        <v>145</v>
+      </c>
+      <c r="L6" s="7">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="M6" s="8">
+        <f t="shared" si="3"/>
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="N6" s="8" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14">
+      <c r="B11" t="s">
+        <v>87</v>
+      </c>
+      <c r="C11" t="s">
+        <v>88</v>
+      </c>
+      <c r="F11" t="s">
+        <v>88</v>
+      </c>
+      <c r="I11" t="s">
+        <v>88</v>
+      </c>
+      <c r="L11" t="s">
+        <v>88</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="C1:E1"/>
+    <mergeCell ref="L1:N1"/>
+    <mergeCell ref="I1:K1"/>
+    <mergeCell ref="F1:H1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
pass get excel file of testcase
</commit_message>
<xml_diff>
--- a/JavaExcelBDD/src/test/resources/ExcelBDD.xlsx
+++ b/JavaExcelBDD/src/test/resources/ExcelBDD.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/2fe8b90741a02718/Git/SimpleOpenExcelBDD/JavaExcelBDD/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="26" documentId="8_{79812025-A047-44C4-86A7-E2AEC82C8710}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{64A75085-CA41-4304-9A96-A479716AD2B7}"/>
+  <xr:revisionPtr revIDLastSave="28" documentId="8_{79812025-A047-44C4-86A7-E2AEC82C8710}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8AD2E8D0-EF7A-4651-8B98-C7E769CDF117}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="6" xr2:uid="{965C72BA-AC7B-4020-96A1-B4855C2F0853}"/>
   </bookViews>
@@ -930,6 +930,10 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -1071,6 +1075,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1086,16 +1096,6 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -1799,66 +1799,66 @@
       <c r="H11" s="7"/>
     </row>
     <row r="12" spans="1:8" ht="45">
-      <c r="A12" s="44">
+      <c r="A12" s="46">
         <v>11</v>
       </c>
       <c r="B12" s="24" t="s">
         <v>89</v>
       </c>
-      <c r="C12" s="47" t="s">
+      <c r="C12" s="49" t="s">
         <v>5</v>
       </c>
-      <c r="D12" s="48" t="s">
+      <c r="D12" s="50" t="s">
         <v>86</v>
       </c>
-      <c r="E12" s="41">
+      <c r="E12" s="43">
         <v>3</v>
       </c>
-      <c r="F12" s="41">
+      <c r="F12" s="43">
         <v>3</v>
       </c>
-      <c r="G12" s="41">
+      <c r="G12" s="43">
         <v>3</v>
       </c>
-      <c r="H12" s="41">
+      <c r="H12" s="43">
         <v>3</v>
       </c>
     </row>
     <row r="13" spans="1:8">
-      <c r="A13" s="45"/>
+      <c r="A13" s="47"/>
       <c r="B13" s="21" t="s">
         <v>97</v>
       </c>
-      <c r="C13" s="47"/>
-      <c r="D13" s="49"/>
-      <c r="E13" s="42"/>
-      <c r="F13" s="42"/>
-      <c r="G13" s="42"/>
-      <c r="H13" s="42"/>
+      <c r="C13" s="49"/>
+      <c r="D13" s="51"/>
+      <c r="E13" s="44"/>
+      <c r="F13" s="44"/>
+      <c r="G13" s="44"/>
+      <c r="H13" s="44"/>
     </row>
     <row r="14" spans="1:8">
-      <c r="A14" s="45"/>
+      <c r="A14" s="47"/>
       <c r="B14" s="21" t="s">
         <v>84</v>
       </c>
-      <c r="C14" s="47"/>
-      <c r="D14" s="49"/>
-      <c r="E14" s="42"/>
-      <c r="F14" s="42"/>
-      <c r="G14" s="42"/>
-      <c r="H14" s="42"/>
+      <c r="C14" s="49"/>
+      <c r="D14" s="51"/>
+      <c r="E14" s="44"/>
+      <c r="F14" s="44"/>
+      <c r="G14" s="44"/>
+      <c r="H14" s="44"/>
     </row>
     <row r="15" spans="1:8">
-      <c r="A15" s="46"/>
+      <c r="A15" s="48"/>
       <c r="B15" s="22" t="s">
         <v>85</v>
       </c>
-      <c r="C15" s="47"/>
-      <c r="D15" s="50"/>
-      <c r="E15" s="43"/>
-      <c r="F15" s="43"/>
-      <c r="G15" s="43"/>
-      <c r="H15" s="43"/>
+      <c r="C15" s="49"/>
+      <c r="D15" s="52"/>
+      <c r="E15" s="45"/>
+      <c r="F15" s="45"/>
+      <c r="G15" s="45"/>
+      <c r="H15" s="45"/>
     </row>
     <row r="16" spans="1:8" ht="30">
       <c r="A16" s="26">
@@ -2040,7 +2040,7 @@
       <c r="G6" s="19"/>
     </row>
     <row r="7" spans="1:7">
-      <c r="A7" s="51" t="s">
+      <c r="A7" s="53" t="s">
         <v>77</v>
       </c>
       <c r="B7" s="4" t="s">
@@ -2053,7 +2053,7 @@
       <c r="G7" s="19"/>
     </row>
     <row r="8" spans="1:7">
-      <c r="A8" s="52"/>
+      <c r="A8" s="54"/>
       <c r="B8" s="4" t="s">
         <v>83</v>
       </c>
@@ -2064,7 +2064,7 @@
       <c r="G8" s="19"/>
     </row>
     <row r="9" spans="1:7">
-      <c r="A9" s="53" t="s">
+      <c r="A9" s="55" t="s">
         <v>78</v>
       </c>
       <c r="B9" s="4" t="s">
@@ -2087,7 +2087,7 @@
       </c>
     </row>
     <row r="10" spans="1:7">
-      <c r="A10" s="54"/>
+      <c r="A10" s="56"/>
       <c r="B10" s="15" t="s">
         <v>83</v>
       </c>
@@ -2359,15 +2359,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="55" t="s">
+      <c r="A1" s="57" t="s">
         <v>43</v>
       </c>
-      <c r="B1" s="55"/>
-      <c r="C1" s="55"/>
-      <c r="D1" s="55"/>
-      <c r="E1" s="55"/>
-      <c r="F1" s="55"/>
-      <c r="G1" s="55"/>
+      <c r="B1" s="57"/>
+      <c r="C1" s="57"/>
+      <c r="D1" s="57"/>
+      <c r="E1" s="57"/>
+      <c r="F1" s="57"/>
+      <c r="G1" s="57"/>
       <c r="H1" s="2"/>
     </row>
     <row r="2" spans="1:8">
@@ -2403,7 +2403,7 @@
       <c r="B3" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="C3" s="56" t="s">
+      <c r="C3" s="58" t="s">
         <v>46</v>
       </c>
       <c r="D3" s="4" t="s">
@@ -2429,7 +2429,7 @@
       <c r="B4" s="9" t="s">
         <v>76</v>
       </c>
-      <c r="C4" s="57"/>
+      <c r="C4" s="59"/>
       <c r="D4" s="4" t="s">
         <v>14</v>
       </c>
@@ -2453,7 +2453,7 @@
       <c r="B5" s="9" t="s">
         <v>77</v>
       </c>
-      <c r="C5" s="58"/>
+      <c r="C5" s="60"/>
       <c r="D5" s="4" t="s">
         <v>15</v>
       </c>
@@ -2531,42 +2531,42 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
-      <c r="A1" s="61" t="s">
+      <c r="A1" s="63" t="s">
         <v>50</v>
       </c>
-      <c r="B1" s="61"/>
-      <c r="C1" s="55" t="s">
+      <c r="B1" s="63"/>
+      <c r="C1" s="57" t="s">
         <v>64</v>
       </c>
-      <c r="D1" s="55"/>
+      <c r="D1" s="57"/>
       <c r="E1" s="14" t="s">
         <v>51</v>
       </c>
-      <c r="F1" s="59" t="s">
+      <c r="F1" s="61" t="s">
         <v>52</v>
       </c>
-      <c r="G1" s="60"/>
-      <c r="H1" s="60"/>
-      <c r="I1" s="60"/>
+      <c r="G1" s="62"/>
+      <c r="H1" s="62"/>
+      <c r="I1" s="62"/>
     </row>
     <row r="2" spans="1:9">
-      <c r="A2" s="61" t="s">
+      <c r="A2" s="63" t="s">
         <v>53</v>
       </c>
-      <c r="B2" s="61"/>
-      <c r="C2" s="67" t="s">
+      <c r="B2" s="63"/>
+      <c r="C2" s="69" t="s">
         <v>49</v>
       </c>
-      <c r="D2" s="67"/>
+      <c r="D2" s="69"/>
       <c r="E2" s="11" t="s">
         <v>80</v>
       </c>
-      <c r="F2" s="65" t="s">
+      <c r="F2" s="67" t="s">
         <v>81</v>
       </c>
-      <c r="G2" s="65"/>
-      <c r="H2" s="65"/>
-      <c r="I2" s="66"/>
+      <c r="G2" s="67"/>
+      <c r="H2" s="67"/>
+      <c r="I2" s="68"/>
     </row>
     <row r="3" spans="1:9">
       <c r="A3" s="13" t="s">
@@ -2598,16 +2598,16 @@
       </c>
     </row>
     <row r="4" spans="1:9" ht="69.95" customHeight="1">
-      <c r="A4" s="62" t="s">
+      <c r="A4" s="64" t="s">
         <v>57</v>
       </c>
       <c r="B4" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="C4" s="62" t="s">
+      <c r="C4" s="64" t="s">
         <v>48</v>
       </c>
-      <c r="D4" s="56" t="s">
+      <c r="D4" s="58" t="s">
         <v>46</v>
       </c>
       <c r="E4" s="4" t="s">
@@ -2627,12 +2627,12 @@
       </c>
     </row>
     <row r="5" spans="1:9" ht="69.95" customHeight="1">
-      <c r="A5" s="63"/>
+      <c r="A5" s="65"/>
       <c r="B5" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="C5" s="63"/>
-      <c r="D5" s="57"/>
+      <c r="C5" s="65"/>
+      <c r="D5" s="59"/>
       <c r="E5" s="4" t="s">
         <v>14</v>
       </c>
@@ -2650,12 +2650,12 @@
       </c>
     </row>
     <row r="6" spans="1:9" ht="69.95" customHeight="1">
-      <c r="A6" s="63"/>
+      <c r="A6" s="65"/>
       <c r="B6" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="C6" s="64"/>
-      <c r="D6" s="58"/>
+      <c r="C6" s="66"/>
+      <c r="D6" s="60"/>
       <c r="E6" s="4" t="s">
         <v>15</v>
       </c>
@@ -2665,7 +2665,7 @@
       <c r="I6" s="8"/>
     </row>
     <row r="7" spans="1:9">
-      <c r="A7" s="64"/>
+      <c r="A7" s="66"/>
       <c r="B7" s="9" t="s">
         <v>61</v>
       </c>
@@ -2749,41 +2749,41 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="23.25">
-      <c r="A1" s="61" t="s">
+      <c r="A1" s="63" t="s">
         <v>50</v>
       </c>
-      <c r="B1" s="61"/>
-      <c r="C1" s="80" t="s">
+      <c r="B1" s="63"/>
+      <c r="C1" s="82" t="s">
         <v>101</v>
       </c>
-      <c r="D1" s="80"/>
-      <c r="E1" s="80"/>
-      <c r="F1" s="80"/>
-      <c r="G1" s="80"/>
-      <c r="H1" s="80"/>
+      <c r="D1" s="82"/>
+      <c r="E1" s="82"/>
+      <c r="F1" s="82"/>
+      <c r="G1" s="82"/>
+      <c r="H1" s="82"/>
     </row>
     <row r="2" spans="1:11" ht="38.25" customHeight="1">
-      <c r="A2" s="85" t="s">
+      <c r="A2" s="87" t="s">
         <v>53</v>
       </c>
-      <c r="B2" s="85"/>
-      <c r="C2" s="81" t="s">
+      <c r="B2" s="87"/>
+      <c r="C2" s="83" t="s">
         <v>102</v>
       </c>
-      <c r="D2" s="81"/>
-      <c r="E2" s="81"/>
-      <c r="F2" s="81"/>
-      <c r="G2" s="81"/>
-      <c r="H2" s="81"/>
+      <c r="D2" s="83"/>
+      <c r="E2" s="83"/>
+      <c r="F2" s="83"/>
+      <c r="G2" s="83"/>
+      <c r="H2" s="83"/>
     </row>
     <row r="3" spans="1:11">
       <c r="A3" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="82" t="s">
+      <c r="B3" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="83"/>
+      <c r="C3" s="85"/>
       <c r="D3" s="13" t="s">
         <v>111</v>
       </c>
@@ -2810,14 +2810,14 @@
       </c>
     </row>
     <row r="4" spans="1:11" ht="15" customHeight="1">
-      <c r="A4" s="62" t="s">
+      <c r="A4" s="64" t="s">
         <v>57</v>
       </c>
-      <c r="B4" s="74" t="s">
+      <c r="B4" s="76" t="s">
         <v>104</v>
       </c>
-      <c r="C4" s="75"/>
-      <c r="D4" s="76"/>
+      <c r="C4" s="77"/>
+      <c r="D4" s="78"/>
       <c r="E4" s="31" t="s">
         <v>103</v>
       </c>
@@ -2841,11 +2841,11 @@
       </c>
     </row>
     <row r="5" spans="1:11" ht="51.75" customHeight="1">
-      <c r="A5" s="63"/>
-      <c r="B5" s="84" t="s">
+      <c r="A5" s="65"/>
+      <c r="B5" s="86" t="s">
         <v>107</v>
       </c>
-      <c r="C5" s="84"/>
+      <c r="C5" s="86"/>
       <c r="D5" s="35" t="s">
         <v>113</v>
       </c>
@@ -2872,12 +2872,12 @@
       </c>
     </row>
     <row r="6" spans="1:11" ht="33.75" customHeight="1">
-      <c r="A6" s="63"/>
-      <c r="B6" s="77" t="s">
+      <c r="A6" s="65"/>
+      <c r="B6" s="79" t="s">
         <v>112</v>
       </c>
-      <c r="C6" s="78"/>
-      <c r="D6" s="79"/>
+      <c r="C6" s="80"/>
+      <c r="D6" s="81"/>
       <c r="E6" s="31" t="s">
         <v>109</v>
       </c>
@@ -2901,11 +2901,11 @@
       </c>
     </row>
     <row r="7" spans="1:11" ht="31.5">
-      <c r="A7" s="63"/>
-      <c r="B7" s="68" t="s">
+      <c r="A7" s="65"/>
+      <c r="B7" s="70" t="s">
         <v>110</v>
       </c>
-      <c r="C7" s="69"/>
+      <c r="C7" s="71"/>
       <c r="D7" s="35" t="s">
         <v>114</v>
       </c>
@@ -2932,9 +2932,9 @@
       </c>
     </row>
     <row r="8" spans="1:11" ht="30">
-      <c r="A8" s="63"/>
-      <c r="B8" s="70"/>
-      <c r="C8" s="71"/>
+      <c r="A8" s="65"/>
+      <c r="B8" s="72"/>
+      <c r="C8" s="73"/>
       <c r="D8" s="36" t="s">
         <v>120</v>
       </c>
@@ -2961,9 +2961,9 @@
       </c>
     </row>
     <row r="9" spans="1:11" ht="31.5">
-      <c r="A9" s="63"/>
-      <c r="B9" s="70"/>
-      <c r="C9" s="71"/>
+      <c r="A9" s="65"/>
+      <c r="B9" s="72"/>
+      <c r="C9" s="73"/>
       <c r="D9" s="35" t="s">
         <v>121</v>
       </c>
@@ -2990,9 +2990,9 @@
       </c>
     </row>
     <row r="10" spans="1:11" ht="31.5">
-      <c r="A10" s="64"/>
-      <c r="B10" s="72"/>
-      <c r="C10" s="73"/>
+      <c r="A10" s="66"/>
+      <c r="B10" s="74"/>
+      <c r="C10" s="75"/>
       <c r="D10" s="35" t="s">
         <v>122</v>
       </c>
@@ -3042,7 +3042,7 @@
   <dimension ref="A3:H13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3058,11 +3058,11 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:8">
-      <c r="F3" s="93" t="s">
+      <c r="F3" s="90" t="s">
         <v>40</v>
       </c>
-      <c r="G3" s="94"/>
-      <c r="H3" s="94"/>
+      <c r="G3" s="91"/>
+      <c r="H3" s="91"/>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" s="6" t="s">
@@ -3091,7 +3091,7 @@
       </c>
     </row>
     <row r="5" spans="1:8">
-      <c r="A5" s="86" t="s">
+      <c r="A5" s="88" t="s">
         <v>28</v>
       </c>
       <c r="B5" s="24" t="s">
@@ -3106,18 +3106,18 @@
       <c r="E5" s="6" t="s">
         <v>148</v>
       </c>
-      <c r="F5" s="95" t="s">
+      <c r="F5" s="41" t="s">
         <v>163</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>164</v>
       </c>
-      <c r="H5" s="96" t="s">
+      <c r="H5" s="42" t="s">
         <v>145</v>
       </c>
     </row>
     <row r="6" spans="1:8">
-      <c r="A6" s="86"/>
+      <c r="A6" s="88"/>
       <c r="B6" s="24" t="s">
         <v>151</v>
       </c>
@@ -3130,18 +3130,18 @@
       <c r="E6" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="F6" s="95" t="s">
+      <c r="F6" s="41" t="s">
         <v>141</v>
       </c>
       <c r="G6" s="2" t="s">
         <v>164</v>
       </c>
-      <c r="H6" s="96" t="s">
+      <c r="H6" s="42" t="s">
         <v>145</v>
       </c>
     </row>
     <row r="7" spans="1:8">
-      <c r="A7" s="86"/>
+      <c r="A7" s="88"/>
       <c r="B7" s="24" t="s">
         <v>25</v>
       </c>
@@ -3154,18 +3154,18 @@
       <c r="E7" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="F7" s="95">
-        <v>1</v>
+      <c r="F7" s="41">
+        <v>2</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>164</v>
-      </c>
-      <c r="H7" s="96" t="s">
+        <v>40</v>
+      </c>
+      <c r="H7" s="42" t="s">
         <v>145</v>
       </c>
     </row>
     <row r="8" spans="1:8">
-      <c r="A8" s="86"/>
+      <c r="A8" s="88"/>
       <c r="B8" s="24" t="s">
         <v>27</v>
       </c>
@@ -3178,18 +3178,18 @@
       <c r="E8" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="F8" s="95" t="s">
+      <c r="F8" s="41" t="s">
         <v>38</v>
       </c>
       <c r="G8" s="2" t="s">
         <v>164</v>
       </c>
-      <c r="H8" s="96" t="s">
+      <c r="H8" s="42" t="s">
         <v>145</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="30">
-      <c r="A9" s="87" t="s">
+      <c r="A9" s="89" t="s">
         <v>152</v>
       </c>
       <c r="B9" s="24" t="s">
@@ -3204,14 +3204,14 @@
       <c r="E9" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="F9" s="95" t="s">
+      <c r="F9" s="41" t="s">
         <v>3</v>
       </c>
       <c r="G9" s="2"/>
-      <c r="H9" s="96"/>
+      <c r="H9" s="42"/>
     </row>
     <row r="10" spans="1:8">
-      <c r="A10" s="87"/>
+      <c r="A10" s="89"/>
       <c r="B10" s="24" t="s">
         <v>153</v>
       </c>
@@ -3224,14 +3224,14 @@
       <c r="E10" s="6" t="s">
         <v>157</v>
       </c>
-      <c r="F10" s="95" t="s">
+      <c r="F10" s="41" t="s">
         <v>17</v>
       </c>
       <c r="G10" s="2"/>
-      <c r="H10" s="96"/>
+      <c r="H10" s="42"/>
     </row>
     <row r="11" spans="1:8">
-      <c r="A11" s="87"/>
+      <c r="A11" s="89"/>
       <c r="B11" s="24" t="s">
         <v>154</v>
       </c>
@@ -3244,14 +3244,14 @@
       <c r="E11" s="6" t="s">
         <v>158</v>
       </c>
-      <c r="F11" s="95">
+      <c r="F11" s="41">
         <v>4.4000000000000004</v>
       </c>
       <c r="G11" s="2"/>
-      <c r="H11" s="96"/>
+      <c r="H11" s="42"/>
     </row>
     <row r="12" spans="1:8">
-      <c r="A12" s="87"/>
+      <c r="A12" s="89"/>
       <c r="B12" s="24" t="s">
         <v>155</v>
       </c>
@@ -3264,14 +3264,14 @@
       <c r="E12" s="6" t="s">
         <v>159</v>
       </c>
-      <c r="F12" s="95" t="s">
+      <c r="F12" s="41" t="s">
         <v>18</v>
       </c>
       <c r="G12" s="2"/>
-      <c r="H12" s="96"/>
+      <c r="H12" s="42"/>
     </row>
     <row r="13" spans="1:8">
-      <c r="A13" s="87"/>
+      <c r="A13" s="89"/>
       <c r="B13" s="25" t="s">
         <v>156</v>
       </c>
@@ -3284,11 +3284,11 @@
       <c r="E13" s="6" t="s">
         <v>161</v>
       </c>
-      <c r="F13" s="95" t="s">
+      <c r="F13" s="41" t="s">
         <v>160</v>
       </c>
       <c r="G13" s="2"/>
-      <c r="H13" s="96"/>
+      <c r="H13" s="42"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -3324,26 +3324,26 @@
       <c r="B1" s="38" t="s">
         <v>146</v>
       </c>
-      <c r="C1" s="88" t="s">
+      <c r="C1" s="92" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="89"/>
-      <c r="E1" s="90"/>
-      <c r="F1" s="88" t="s">
+      <c r="D1" s="93"/>
+      <c r="E1" s="94"/>
+      <c r="F1" s="92" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="89"/>
-      <c r="H1" s="90"/>
-      <c r="I1" s="88" t="s">
+      <c r="G1" s="93"/>
+      <c r="H1" s="94"/>
+      <c r="I1" s="92" t="s">
         <v>65</v>
       </c>
-      <c r="J1" s="89"/>
-      <c r="K1" s="90"/>
-      <c r="L1" s="91" t="s">
+      <c r="J1" s="93"/>
+      <c r="K1" s="94"/>
+      <c r="L1" s="95" t="s">
         <v>66</v>
       </c>
-      <c r="M1" s="92"/>
-      <c r="N1" s="92"/>
+      <c r="M1" s="96"/>
+      <c r="N1" s="96"/>
     </row>
     <row r="2" spans="1:14">
       <c r="A2" s="4" t="s">

</xml_diff>

<commit_message>
refine tech debt in ZMExcel.java
</commit_message>
<xml_diff>
--- a/JavaExcelBDD/src/test/resources/ExcelBDD.xlsx
+++ b/JavaExcelBDD/src/test/resources/ExcelBDD.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/2fe8b90741a02718/Git/SimpleOpenExcelBDD/JavaExcelBDD/src/test/resources/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mike\git\ExcelBDD\JavaExcelBDD\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="28" documentId="8_{79812025-A047-44C4-86A7-E2AEC82C8710}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8AD2E8D0-EF7A-4651-8B98-C7E769CDF117}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BC08F18-7250-451B-B716-B852607D4077}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="7" xr2:uid="{965C72BA-AC7B-4020-96A1-B4855C2F0853}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="395" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="397" uniqueCount="165">
   <si>
     <t>Role</t>
   </si>
@@ -3305,7 +3305,7 @@
   <dimension ref="A1:N11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3568,6 +3568,12 @@
       <c r="C11" t="s">
         <v>88</v>
       </c>
+      <c r="D11" t="s">
+        <v>88</v>
+      </c>
+      <c r="E11" t="s">
+        <v>88</v>
+      </c>
       <c r="F11" t="s">
         <v>88</v>
       </c>

</xml_diff>

<commit_message>
check 1st testcase dataset
</commit_message>
<xml_diff>
--- a/JavaExcelBDD/src/test/resources/ExcelBDD.xlsx
+++ b/JavaExcelBDD/src/test/resources/ExcelBDD.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mike\git\ExcelBDD\JavaExcelBDD\src\test\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/2fe8b90741a02718/Git/SimpleOpenExcelBDD/JavaExcelBDD/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BC08F18-7250-451B-B716-B852607D4077}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
@@ -3305,7 +3305,7 @@
   <dimension ref="A1:N11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>

<commit_message>
fix bug of mapTestSetHeader sequence
</commit_message>
<xml_diff>
--- a/JavaExcelBDD/src/test/resources/ExcelBDD.xlsx
+++ b/JavaExcelBDD/src/test/resources/ExcelBDD.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/2fe8b90741a02718/Git/SimpleOpenExcelBDD/JavaExcelBDD/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="8" documentId="13_ncr:1_{2BC08F18-7250-451B-B716-B852607D4077}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A76B4D93-EE20-443C-9598-C23B5321E18B}"/>
+  <xr:revisionPtr revIDLastSave="43" documentId="13_ncr:1_{2BC08F18-7250-451B-B716-B852607D4077}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6E37B364-7A12-4803-B6B2-14C59C4D0115}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="8" xr2:uid="{965C72BA-AC7B-4020-96A1-B4855C2F0853}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="9" xr2:uid="{965C72BA-AC7B-4020-96A1-B4855C2F0853}"/>
   </bookViews>
   <sheets>
     <sheet name="SimpleOpenBDD" sheetId="1" r:id="rId1"/>
@@ -22,6 +22,8 @@
     <sheet name="SpecificationByTestcase" sheetId="9" r:id="rId7"/>
     <sheet name="SBTSheet1" sheetId="7" r:id="rId8"/>
     <sheet name="SBTSheet2" sheetId="10" r:id="rId9"/>
+    <sheet name="SBTSheet3" sheetId="11" r:id="rId10"/>
+    <sheet name="SBTSheet3 (2)" sheetId="12" r:id="rId11"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -42,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="458" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="620" uniqueCount="168">
   <si>
     <t>Role</t>
   </si>
@@ -538,6 +540,15 @@
   </si>
   <si>
     <t>got</t>
+  </si>
+  <si>
+    <t>GUI Prototype</t>
+  </si>
+  <si>
+    <t>V1.6</t>
+  </si>
+  <si>
+    <t>V2.6</t>
   </si>
 </sst>
 </file>
@@ -845,7 +856,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="98">
+  <cellXfs count="99">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -935,6 +946,7 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -1097,7 +1109,9 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -1203,6 +1217,104 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="1857375" y="485775"/>
+          <a:ext cx="2932542" cy="2276475"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>276225</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>3208767</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>2400300</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="图片 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3343CC5A-23AA-4074-A67D-FD3335DE981A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2419350" y="695325"/>
+          <a:ext cx="2932542" cy="2276475"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>276225</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>3208767</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>2400300</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="图片 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2F385B2A-A2CD-43B8-A7C4-46F10268F5C4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2419350" y="1076325"/>
           <a:ext cx="2932542" cy="2276475"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1801,66 +1913,66 @@
       <c r="H11" s="7"/>
     </row>
     <row r="12" spans="1:8" ht="45">
-      <c r="A12" s="46">
+      <c r="A12" s="47">
         <v>11</v>
       </c>
       <c r="B12" s="24" t="s">
         <v>89</v>
       </c>
-      <c r="C12" s="49" t="s">
+      <c r="C12" s="50" t="s">
         <v>5</v>
       </c>
-      <c r="D12" s="50" t="s">
+      <c r="D12" s="51" t="s">
         <v>86</v>
       </c>
-      <c r="E12" s="43">
+      <c r="E12" s="44">
         <v>3</v>
       </c>
-      <c r="F12" s="43">
+      <c r="F12" s="44">
         <v>3</v>
       </c>
-      <c r="G12" s="43">
+      <c r="G12" s="44">
         <v>3</v>
       </c>
-      <c r="H12" s="43">
+      <c r="H12" s="44">
         <v>3</v>
       </c>
     </row>
     <row r="13" spans="1:8">
-      <c r="A13" s="47"/>
+      <c r="A13" s="48"/>
       <c r="B13" s="21" t="s">
         <v>97</v>
       </c>
-      <c r="C13" s="49"/>
-      <c r="D13" s="51"/>
-      <c r="E13" s="44"/>
-      <c r="F13" s="44"/>
-      <c r="G13" s="44"/>
-      <c r="H13" s="44"/>
+      <c r="C13" s="50"/>
+      <c r="D13" s="52"/>
+      <c r="E13" s="45"/>
+      <c r="F13" s="45"/>
+      <c r="G13" s="45"/>
+      <c r="H13" s="45"/>
     </row>
     <row r="14" spans="1:8">
-      <c r="A14" s="47"/>
+      <c r="A14" s="48"/>
       <c r="B14" s="21" t="s">
         <v>84</v>
       </c>
-      <c r="C14" s="49"/>
-      <c r="D14" s="51"/>
-      <c r="E14" s="44"/>
-      <c r="F14" s="44"/>
-      <c r="G14" s="44"/>
-      <c r="H14" s="44"/>
+      <c r="C14" s="50"/>
+      <c r="D14" s="52"/>
+      <c r="E14" s="45"/>
+      <c r="F14" s="45"/>
+      <c r="G14" s="45"/>
+      <c r="H14" s="45"/>
     </row>
     <row r="15" spans="1:8">
-      <c r="A15" s="48"/>
+      <c r="A15" s="49"/>
       <c r="B15" s="22" t="s">
         <v>85</v>
       </c>
-      <c r="C15" s="49"/>
-      <c r="D15" s="52"/>
-      <c r="E15" s="45"/>
-      <c r="F15" s="45"/>
-      <c r="G15" s="45"/>
-      <c r="H15" s="45"/>
+      <c r="C15" s="50"/>
+      <c r="D15" s="53"/>
+      <c r="E15" s="46"/>
+      <c r="F15" s="46"/>
+      <c r="G15" s="46"/>
+      <c r="H15" s="46"/>
     </row>
     <row r="16" spans="1:8" ht="30">
       <c r="A16" s="26">
@@ -1926,6 +2038,795 @@
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27202F44-224C-40C0-ACC3-02135A9560D7}">
+  <dimension ref="A1:V11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="T7" sqref="T7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="23" customWidth="1"/>
+    <col min="3" max="3" width="53.85546875" customWidth="1"/>
+    <col min="4" max="4" width="25.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.7109375" customWidth="1"/>
+    <col min="7" max="7" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="10.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:22">
+      <c r="D1" s="38" t="s">
+        <v>146</v>
+      </c>
+      <c r="E1" s="93" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="94"/>
+      <c r="G1" s="95"/>
+      <c r="H1" s="93" t="s">
+        <v>4</v>
+      </c>
+      <c r="I1" s="94"/>
+      <c r="J1" s="95"/>
+      <c r="K1" s="93" t="s">
+        <v>65</v>
+      </c>
+      <c r="L1" s="94"/>
+      <c r="M1" s="95"/>
+      <c r="N1" s="98" t="s">
+        <v>66</v>
+      </c>
+      <c r="O1" s="98"/>
+      <c r="P1" s="98"/>
+      <c r="Q1" s="93" t="s">
+        <v>131</v>
+      </c>
+      <c r="R1" s="94"/>
+      <c r="S1" s="95"/>
+      <c r="T1" s="93" t="s">
+        <v>132</v>
+      </c>
+      <c r="U1" s="94"/>
+      <c r="V1" s="95"/>
+    </row>
+    <row r="2" spans="1:22">
+      <c r="A2" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="E2" s="37" t="s">
+        <v>142</v>
+      </c>
+      <c r="F2" s="37" t="s">
+        <v>143</v>
+      </c>
+      <c r="G2" s="37" t="s">
+        <v>144</v>
+      </c>
+      <c r="H2" s="37" t="s">
+        <v>142</v>
+      </c>
+      <c r="I2" s="37" t="s">
+        <v>143</v>
+      </c>
+      <c r="J2" s="37" t="s">
+        <v>144</v>
+      </c>
+      <c r="K2" s="37" t="s">
+        <v>142</v>
+      </c>
+      <c r="L2" s="37" t="s">
+        <v>143</v>
+      </c>
+      <c r="M2" s="37" t="s">
+        <v>144</v>
+      </c>
+      <c r="N2" s="37" t="s">
+        <v>142</v>
+      </c>
+      <c r="O2" s="37" t="s">
+        <v>143</v>
+      </c>
+      <c r="P2" s="37" t="s">
+        <v>144</v>
+      </c>
+      <c r="Q2" s="37" t="s">
+        <v>142</v>
+      </c>
+      <c r="R2" s="37" t="s">
+        <v>143</v>
+      </c>
+      <c r="S2" s="37" t="s">
+        <v>144</v>
+      </c>
+      <c r="T2" s="37" t="s">
+        <v>142</v>
+      </c>
+      <c r="U2" s="37" t="s">
+        <v>143</v>
+      </c>
+      <c r="V2" s="37" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="3" spans="1:22">
+      <c r="A3" s="9">
+        <v>1</v>
+      </c>
+      <c r="B3" s="23" t="s">
+        <v>75</v>
+      </c>
+      <c r="C3" s="23"/>
+      <c r="D3" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="F3" s="8" t="str">
+        <f>E3</f>
+        <v>V1.1</v>
+      </c>
+      <c r="G3" s="8" t="s">
+        <v>145</v>
+      </c>
+      <c r="H3" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="I3" s="8" t="str">
+        <f>H3</f>
+        <v>V1.2</v>
+      </c>
+      <c r="J3" s="8" t="s">
+        <v>145</v>
+      </c>
+      <c r="K3" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="L3" s="8" t="str">
+        <f>K3</f>
+        <v>V1.3</v>
+      </c>
+      <c r="M3" s="8" t="s">
+        <v>145</v>
+      </c>
+      <c r="N3" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="O3" s="8" t="str">
+        <f>N3</f>
+        <v>V1.4</v>
+      </c>
+      <c r="P3" s="8" t="s">
+        <v>145</v>
+      </c>
+      <c r="Q3" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="R3" s="8" t="str">
+        <f>Q3</f>
+        <v>V1.5</v>
+      </c>
+      <c r="S3" s="8" t="s">
+        <v>145</v>
+      </c>
+      <c r="T3" s="8" t="s">
+        <v>166</v>
+      </c>
+      <c r="U3" s="8" t="str">
+        <f>T3</f>
+        <v>V1.6</v>
+      </c>
+      <c r="V3" s="8" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22" ht="214.5" customHeight="1">
+      <c r="A4" s="9">
+        <v>2</v>
+      </c>
+      <c r="B4" s="23" t="s">
+        <v>76</v>
+      </c>
+      <c r="C4" s="23"/>
+      <c r="D4" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="F4" s="8" t="str">
+        <f t="shared" ref="F4:F6" si="0">E4</f>
+        <v>V2.1</v>
+      </c>
+      <c r="G4" s="8" t="s">
+        <v>145</v>
+      </c>
+      <c r="H4" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="I4" s="8" t="str">
+        <f t="shared" ref="I4:I6" si="1">H4</f>
+        <v>V2.2</v>
+      </c>
+      <c r="J4" s="8" t="s">
+        <v>145</v>
+      </c>
+      <c r="K4" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="L4" s="8" t="str">
+        <f t="shared" ref="L4:L6" si="2">K4</f>
+        <v>V2.3</v>
+      </c>
+      <c r="M4" s="8" t="s">
+        <v>145</v>
+      </c>
+      <c r="N4" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="O4" s="8" t="str">
+        <f t="shared" ref="O4:O6" si="3">N4</f>
+        <v>V2.4</v>
+      </c>
+      <c r="P4" s="8" t="s">
+        <v>145</v>
+      </c>
+      <c r="Q4" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="R4" s="8" t="str">
+        <f t="shared" ref="R4" si="4">Q4</f>
+        <v>V2.5</v>
+      </c>
+      <c r="S4" s="8" t="s">
+        <v>145</v>
+      </c>
+      <c r="T4" s="8" t="s">
+        <v>167</v>
+      </c>
+      <c r="U4" s="8" t="str">
+        <f t="shared" ref="U4" si="5">T4</f>
+        <v>V2.6</v>
+      </c>
+      <c r="V4" s="8" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22">
+      <c r="A5" s="9">
+        <v>3</v>
+      </c>
+      <c r="B5" s="39" t="s">
+        <v>77</v>
+      </c>
+      <c r="C5" s="39"/>
+      <c r="D5" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5" s="8"/>
+      <c r="F5" s="8"/>
+      <c r="G5" s="8" t="s">
+        <v>145</v>
+      </c>
+      <c r="H5" s="8"/>
+      <c r="I5" s="8"/>
+      <c r="J5" s="8" t="s">
+        <v>145</v>
+      </c>
+      <c r="K5" s="8"/>
+      <c r="L5" s="8"/>
+      <c r="M5" s="8" t="s">
+        <v>145</v>
+      </c>
+      <c r="N5" s="8"/>
+      <c r="O5" s="8"/>
+      <c r="P5" s="8" t="s">
+        <v>145</v>
+      </c>
+      <c r="Q5" s="8"/>
+      <c r="R5" s="8"/>
+      <c r="S5" s="8" t="s">
+        <v>145</v>
+      </c>
+      <c r="T5" s="8"/>
+      <c r="U5" s="8"/>
+      <c r="V5" s="8" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22">
+      <c r="A6" s="9">
+        <v>4</v>
+      </c>
+      <c r="B6" s="40" t="s">
+        <v>78</v>
+      </c>
+      <c r="C6" s="40"/>
+      <c r="D6" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E6" s="30" t="s">
+        <v>100</v>
+      </c>
+      <c r="F6" s="8" t="str">
+        <f t="shared" si="0"/>
+        <v>2021/4/30</v>
+      </c>
+      <c r="G6" s="8" t="s">
+        <v>145</v>
+      </c>
+      <c r="H6" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="I6" s="8" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J6" s="8" t="s">
+        <v>145</v>
+      </c>
+      <c r="K6" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="L6" s="8" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="M6" s="8" t="s">
+        <v>145</v>
+      </c>
+      <c r="N6" s="7">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="O6" s="8">
+        <f t="shared" si="3"/>
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="P6" s="8" t="s">
+        <v>145</v>
+      </c>
+      <c r="Q6" s="7">
+        <v>4.5</v>
+      </c>
+      <c r="R6" s="8">
+        <f t="shared" ref="R6" si="6">Q6</f>
+        <v>4.5</v>
+      </c>
+      <c r="S6" s="8" t="s">
+        <v>145</v>
+      </c>
+      <c r="T6" s="7">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="U6" s="8">
+        <f t="shared" ref="U6" si="7">T6</f>
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="V6" s="8" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="11" spans="1:22">
+      <c r="D11" t="s">
+        <v>87</v>
+      </c>
+      <c r="E11" t="s">
+        <v>88</v>
+      </c>
+      <c r="F11" t="s">
+        <v>88</v>
+      </c>
+      <c r="G11" t="s">
+        <v>88</v>
+      </c>
+      <c r="H11" t="s">
+        <v>88</v>
+      </c>
+      <c r="K11" t="s">
+        <v>88</v>
+      </c>
+      <c r="N11" t="s">
+        <v>88</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="T1:V1"/>
+    <mergeCell ref="E1:G1"/>
+    <mergeCell ref="H1:J1"/>
+    <mergeCell ref="K1:M1"/>
+    <mergeCell ref="N1:P1"/>
+    <mergeCell ref="Q1:S1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B2264DA-2ABC-4703-92C5-C6046C9B8A71}">
+  <dimension ref="A3:S13"/>
+  <sheetViews>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="Q3" sqref="Q3:S8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="23" customWidth="1"/>
+    <col min="3" max="3" width="53.85546875" customWidth="1"/>
+    <col min="4" max="4" width="25.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.7109375" customWidth="1"/>
+    <col min="7" max="7" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="10.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:19">
+      <c r="D3" s="38" t="s">
+        <v>146</v>
+      </c>
+      <c r="E3" s="93" t="s">
+        <v>3</v>
+      </c>
+      <c r="F3" s="94"/>
+      <c r="G3" s="95"/>
+      <c r="H3" s="93" t="s">
+        <v>4</v>
+      </c>
+      <c r="I3" s="94"/>
+      <c r="J3" s="95"/>
+      <c r="K3" s="93" t="s">
+        <v>65</v>
+      </c>
+      <c r="L3" s="94"/>
+      <c r="M3" s="95"/>
+      <c r="N3" s="98" t="s">
+        <v>66</v>
+      </c>
+      <c r="O3" s="98"/>
+      <c r="P3" s="98"/>
+      <c r="Q3" s="93" t="s">
+        <v>131</v>
+      </c>
+      <c r="R3" s="94"/>
+      <c r="S3" s="95"/>
+    </row>
+    <row r="4" spans="1:19">
+      <c r="A4" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="E4" s="37" t="s">
+        <v>142</v>
+      </c>
+      <c r="F4" s="37" t="s">
+        <v>143</v>
+      </c>
+      <c r="G4" s="37" t="s">
+        <v>144</v>
+      </c>
+      <c r="H4" s="37" t="s">
+        <v>142</v>
+      </c>
+      <c r="I4" s="37" t="s">
+        <v>143</v>
+      </c>
+      <c r="J4" s="37" t="s">
+        <v>144</v>
+      </c>
+      <c r="K4" s="37" t="s">
+        <v>142</v>
+      </c>
+      <c r="L4" s="37" t="s">
+        <v>143</v>
+      </c>
+      <c r="M4" s="37" t="s">
+        <v>144</v>
+      </c>
+      <c r="N4" s="37" t="s">
+        <v>142</v>
+      </c>
+      <c r="O4" s="37" t="s">
+        <v>143</v>
+      </c>
+      <c r="P4" s="37" t="s">
+        <v>144</v>
+      </c>
+      <c r="Q4" s="37" t="s">
+        <v>142</v>
+      </c>
+      <c r="R4" s="37" t="s">
+        <v>143</v>
+      </c>
+      <c r="S4" s="37" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19">
+      <c r="A5" s="9">
+        <v>1</v>
+      </c>
+      <c r="B5" s="23" t="s">
+        <v>75</v>
+      </c>
+      <c r="C5" s="23"/>
+      <c r="D5" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="F5" s="8" t="str">
+        <f>E5</f>
+        <v>V1.1</v>
+      </c>
+      <c r="G5" s="8" t="s">
+        <v>145</v>
+      </c>
+      <c r="H5" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="I5" s="8" t="str">
+        <f>H5</f>
+        <v>V1.2</v>
+      </c>
+      <c r="J5" s="8" t="s">
+        <v>145</v>
+      </c>
+      <c r="K5" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="L5" s="8" t="str">
+        <f>K5</f>
+        <v>V1.3</v>
+      </c>
+      <c r="M5" s="8" t="s">
+        <v>145</v>
+      </c>
+      <c r="N5" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="O5" s="8" t="str">
+        <f>N5</f>
+        <v>V1.4</v>
+      </c>
+      <c r="P5" s="8" t="s">
+        <v>145</v>
+      </c>
+      <c r="Q5" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="R5" s="8" t="str">
+        <f>Q5</f>
+        <v>V1.5</v>
+      </c>
+      <c r="S5" s="8" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" ht="214.5" customHeight="1">
+      <c r="A6" s="9">
+        <v>2</v>
+      </c>
+      <c r="B6" s="23" t="s">
+        <v>76</v>
+      </c>
+      <c r="C6" s="23"/>
+      <c r="D6" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="F6" s="8" t="str">
+        <f t="shared" ref="F6:F8" si="0">E6</f>
+        <v>V2.1</v>
+      </c>
+      <c r="G6" s="8" t="s">
+        <v>145</v>
+      </c>
+      <c r="H6" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="I6" s="8" t="str">
+        <f t="shared" ref="I6:I8" si="1">H6</f>
+        <v>V2.2</v>
+      </c>
+      <c r="J6" s="8" t="s">
+        <v>145</v>
+      </c>
+      <c r="K6" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="L6" s="8" t="str">
+        <f t="shared" ref="L6:L8" si="2">K6</f>
+        <v>V2.3</v>
+      </c>
+      <c r="M6" s="8" t="s">
+        <v>145</v>
+      </c>
+      <c r="N6" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="O6" s="8" t="str">
+        <f t="shared" ref="O6:O8" si="3">N6</f>
+        <v>V2.4</v>
+      </c>
+      <c r="P6" s="8" t="s">
+        <v>145</v>
+      </c>
+      <c r="Q6" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="R6" s="8" t="str">
+        <f t="shared" ref="R6" si="4">Q6</f>
+        <v>V2.5</v>
+      </c>
+      <c r="S6" s="8" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19">
+      <c r="A7" s="9">
+        <v>3</v>
+      </c>
+      <c r="B7" s="39" t="s">
+        <v>77</v>
+      </c>
+      <c r="C7" s="39"/>
+      <c r="D7" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E7" s="8"/>
+      <c r="F7" s="8"/>
+      <c r="G7" s="8" t="s">
+        <v>145</v>
+      </c>
+      <c r="H7" s="8"/>
+      <c r="I7" s="8"/>
+      <c r="J7" s="8" t="s">
+        <v>145</v>
+      </c>
+      <c r="K7" s="8"/>
+      <c r="L7" s="8"/>
+      <c r="M7" s="8" t="s">
+        <v>145</v>
+      </c>
+      <c r="N7" s="8"/>
+      <c r="O7" s="8"/>
+      <c r="P7" s="8" t="s">
+        <v>145</v>
+      </c>
+      <c r="Q7" s="8"/>
+      <c r="R7" s="8"/>
+      <c r="S7" s="8" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19">
+      <c r="A8" s="9">
+        <v>4</v>
+      </c>
+      <c r="B8" s="40" t="s">
+        <v>78</v>
+      </c>
+      <c r="C8" s="40"/>
+      <c r="D8" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E8" s="30" t="s">
+        <v>100</v>
+      </c>
+      <c r="F8" s="8" t="str">
+        <f t="shared" si="0"/>
+        <v>2021/4/30</v>
+      </c>
+      <c r="G8" s="8" t="s">
+        <v>145</v>
+      </c>
+      <c r="H8" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="I8" s="8" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J8" s="8" t="s">
+        <v>145</v>
+      </c>
+      <c r="K8" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="L8" s="8" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="M8" s="8" t="s">
+        <v>145</v>
+      </c>
+      <c r="N8" s="7">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="O8" s="8">
+        <f t="shared" si="3"/>
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="P8" s="8" t="s">
+        <v>145</v>
+      </c>
+      <c r="Q8" s="7">
+        <v>5.4</v>
+      </c>
+      <c r="R8" s="8">
+        <f t="shared" ref="R8" si="5">Q8</f>
+        <v>5.4</v>
+      </c>
+      <c r="S8" s="8" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19">
+      <c r="D13" t="s">
+        <v>87</v>
+      </c>
+      <c r="E13" t="s">
+        <v>88</v>
+      </c>
+      <c r="F13" t="s">
+        <v>88</v>
+      </c>
+      <c r="G13" t="s">
+        <v>88</v>
+      </c>
+      <c r="H13" t="s">
+        <v>88</v>
+      </c>
+      <c r="K13" t="s">
+        <v>88</v>
+      </c>
+      <c r="N13" t="s">
+        <v>88</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="E3:G3"/>
+    <mergeCell ref="H3:J3"/>
+    <mergeCell ref="K3:M3"/>
+    <mergeCell ref="N3:P3"/>
+    <mergeCell ref="Q3:S3"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2042,7 +2943,7 @@
       <c r="G6" s="19"/>
     </row>
     <row r="7" spans="1:7">
-      <c r="A7" s="53" t="s">
+      <c r="A7" s="54" t="s">
         <v>77</v>
       </c>
       <c r="B7" s="4" t="s">
@@ -2055,7 +2956,7 @@
       <c r="G7" s="19"/>
     </row>
     <row r="8" spans="1:7">
-      <c r="A8" s="54"/>
+      <c r="A8" s="55"/>
       <c r="B8" s="4" t="s">
         <v>83</v>
       </c>
@@ -2066,7 +2967,7 @@
       <c r="G8" s="19"/>
     </row>
     <row r="9" spans="1:7">
-      <c r="A9" s="55" t="s">
+      <c r="A9" s="56" t="s">
         <v>78</v>
       </c>
       <c r="B9" s="4" t="s">
@@ -2089,7 +2990,7 @@
       </c>
     </row>
     <row r="10" spans="1:7">
-      <c r="A10" s="56"/>
+      <c r="A10" s="57"/>
       <c r="B10" s="15" t="s">
         <v>83</v>
       </c>
@@ -2349,7 +3250,7 @@
   <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="A2" sqref="A2:A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2361,15 +3262,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="57" t="s">
+      <c r="A1" s="58" t="s">
         <v>43</v>
       </c>
-      <c r="B1" s="57"/>
-      <c r="C1" s="57"/>
-      <c r="D1" s="57"/>
-      <c r="E1" s="57"/>
-      <c r="F1" s="57"/>
-      <c r="G1" s="57"/>
+      <c r="B1" s="58"/>
+      <c r="C1" s="58"/>
+      <c r="D1" s="58"/>
+      <c r="E1" s="58"/>
+      <c r="F1" s="58"/>
+      <c r="G1" s="58"/>
       <c r="H1" s="2"/>
     </row>
     <row r="2" spans="1:8">
@@ -2405,7 +3306,7 @@
       <c r="B3" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="C3" s="58" t="s">
+      <c r="C3" s="59" t="s">
         <v>46</v>
       </c>
       <c r="D3" s="4" t="s">
@@ -2431,7 +3332,7 @@
       <c r="B4" s="9" t="s">
         <v>76</v>
       </c>
-      <c r="C4" s="59"/>
+      <c r="C4" s="60"/>
       <c r="D4" s="4" t="s">
         <v>14</v>
       </c>
@@ -2455,7 +3356,7 @@
       <c r="B5" s="9" t="s">
         <v>77</v>
       </c>
-      <c r="C5" s="60"/>
+      <c r="C5" s="61"/>
       <c r="D5" s="4" t="s">
         <v>15</v>
       </c>
@@ -2533,42 +3434,42 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
-      <c r="A1" s="63" t="s">
+      <c r="A1" s="64" t="s">
         <v>50</v>
       </c>
-      <c r="B1" s="63"/>
-      <c r="C1" s="57" t="s">
+      <c r="B1" s="64"/>
+      <c r="C1" s="58" t="s">
         <v>64</v>
       </c>
-      <c r="D1" s="57"/>
+      <c r="D1" s="58"/>
       <c r="E1" s="14" t="s">
         <v>51</v>
       </c>
-      <c r="F1" s="61" t="s">
+      <c r="F1" s="62" t="s">
         <v>52</v>
       </c>
-      <c r="G1" s="62"/>
-      <c r="H1" s="62"/>
-      <c r="I1" s="62"/>
+      <c r="G1" s="63"/>
+      <c r="H1" s="63"/>
+      <c r="I1" s="63"/>
     </row>
     <row r="2" spans="1:9">
-      <c r="A2" s="63" t="s">
+      <c r="A2" s="64" t="s">
         <v>53</v>
       </c>
-      <c r="B2" s="63"/>
-      <c r="C2" s="69" t="s">
+      <c r="B2" s="64"/>
+      <c r="C2" s="70" t="s">
         <v>49</v>
       </c>
-      <c r="D2" s="69"/>
+      <c r="D2" s="70"/>
       <c r="E2" s="11" t="s">
         <v>80</v>
       </c>
-      <c r="F2" s="67" t="s">
+      <c r="F2" s="68" t="s">
         <v>81</v>
       </c>
-      <c r="G2" s="67"/>
-      <c r="H2" s="67"/>
-      <c r="I2" s="68"/>
+      <c r="G2" s="68"/>
+      <c r="H2" s="68"/>
+      <c r="I2" s="69"/>
     </row>
     <row r="3" spans="1:9">
       <c r="A3" s="13" t="s">
@@ -2600,16 +3501,16 @@
       </c>
     </row>
     <row r="4" spans="1:9" ht="69.95" customHeight="1">
-      <c r="A4" s="64" t="s">
+      <c r="A4" s="65" t="s">
         <v>57</v>
       </c>
       <c r="B4" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="C4" s="64" t="s">
+      <c r="C4" s="65" t="s">
         <v>48</v>
       </c>
-      <c r="D4" s="58" t="s">
+      <c r="D4" s="59" t="s">
         <v>46</v>
       </c>
       <c r="E4" s="4" t="s">
@@ -2629,12 +3530,12 @@
       </c>
     </row>
     <row r="5" spans="1:9" ht="69.95" customHeight="1">
-      <c r="A5" s="65"/>
+      <c r="A5" s="66"/>
       <c r="B5" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="C5" s="65"/>
-      <c r="D5" s="59"/>
+      <c r="C5" s="66"/>
+      <c r="D5" s="60"/>
       <c r="E5" s="4" t="s">
         <v>14</v>
       </c>
@@ -2652,12 +3553,12 @@
       </c>
     </row>
     <row r="6" spans="1:9" ht="69.95" customHeight="1">
-      <c r="A6" s="65"/>
+      <c r="A6" s="66"/>
       <c r="B6" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="C6" s="66"/>
-      <c r="D6" s="60"/>
+      <c r="C6" s="67"/>
+      <c r="D6" s="61"/>
       <c r="E6" s="4" t="s">
         <v>15</v>
       </c>
@@ -2667,7 +3568,7 @@
       <c r="I6" s="8"/>
     </row>
     <row r="7" spans="1:9">
-      <c r="A7" s="66"/>
+      <c r="A7" s="67"/>
       <c r="B7" s="9" t="s">
         <v>61</v>
       </c>
@@ -2751,41 +3652,41 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="23.25">
-      <c r="A1" s="63" t="s">
+      <c r="A1" s="64" t="s">
         <v>50</v>
       </c>
-      <c r="B1" s="63"/>
-      <c r="C1" s="82" t="s">
+      <c r="B1" s="64"/>
+      <c r="C1" s="83" t="s">
         <v>101</v>
       </c>
-      <c r="D1" s="82"/>
-      <c r="E1" s="82"/>
-      <c r="F1" s="82"/>
-      <c r="G1" s="82"/>
-      <c r="H1" s="82"/>
+      <c r="D1" s="83"/>
+      <c r="E1" s="83"/>
+      <c r="F1" s="83"/>
+      <c r="G1" s="83"/>
+      <c r="H1" s="83"/>
     </row>
     <row r="2" spans="1:11" ht="38.25" customHeight="1">
-      <c r="A2" s="87" t="s">
+      <c r="A2" s="88" t="s">
         <v>53</v>
       </c>
-      <c r="B2" s="87"/>
-      <c r="C2" s="83" t="s">
+      <c r="B2" s="88"/>
+      <c r="C2" s="84" t="s">
         <v>102</v>
       </c>
-      <c r="D2" s="83"/>
-      <c r="E2" s="83"/>
-      <c r="F2" s="83"/>
-      <c r="G2" s="83"/>
-      <c r="H2" s="83"/>
+      <c r="D2" s="84"/>
+      <c r="E2" s="84"/>
+      <c r="F2" s="84"/>
+      <c r="G2" s="84"/>
+      <c r="H2" s="84"/>
     </row>
     <row r="3" spans="1:11">
       <c r="A3" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="84" t="s">
+      <c r="B3" s="85" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="85"/>
+      <c r="C3" s="86"/>
       <c r="D3" s="13" t="s">
         <v>111</v>
       </c>
@@ -2812,14 +3713,14 @@
       </c>
     </row>
     <row r="4" spans="1:11" ht="15" customHeight="1">
-      <c r="A4" s="64" t="s">
+      <c r="A4" s="65" t="s">
         <v>57</v>
       </c>
-      <c r="B4" s="76" t="s">
+      <c r="B4" s="77" t="s">
         <v>104</v>
       </c>
-      <c r="C4" s="77"/>
-      <c r="D4" s="78"/>
+      <c r="C4" s="78"/>
+      <c r="D4" s="79"/>
       <c r="E4" s="31" t="s">
         <v>103</v>
       </c>
@@ -2843,11 +3744,11 @@
       </c>
     </row>
     <row r="5" spans="1:11" ht="51.75" customHeight="1">
-      <c r="A5" s="65"/>
-      <c r="B5" s="86" t="s">
+      <c r="A5" s="66"/>
+      <c r="B5" s="87" t="s">
         <v>107</v>
       </c>
-      <c r="C5" s="86"/>
+      <c r="C5" s="87"/>
       <c r="D5" s="35" t="s">
         <v>113</v>
       </c>
@@ -2874,12 +3775,12 @@
       </c>
     </row>
     <row r="6" spans="1:11" ht="33.75" customHeight="1">
-      <c r="A6" s="65"/>
-      <c r="B6" s="79" t="s">
+      <c r="A6" s="66"/>
+      <c r="B6" s="80" t="s">
         <v>112</v>
       </c>
-      <c r="C6" s="80"/>
-      <c r="D6" s="81"/>
+      <c r="C6" s="81"/>
+      <c r="D6" s="82"/>
       <c r="E6" s="31" t="s">
         <v>109</v>
       </c>
@@ -2903,11 +3804,11 @@
       </c>
     </row>
     <row r="7" spans="1:11" ht="31.5">
-      <c r="A7" s="65"/>
-      <c r="B7" s="70" t="s">
+      <c r="A7" s="66"/>
+      <c r="B7" s="71" t="s">
         <v>110</v>
       </c>
-      <c r="C7" s="71"/>
+      <c r="C7" s="72"/>
       <c r="D7" s="35" t="s">
         <v>114</v>
       </c>
@@ -2934,9 +3835,9 @@
       </c>
     </row>
     <row r="8" spans="1:11" ht="30">
-      <c r="A8" s="65"/>
-      <c r="B8" s="72"/>
-      <c r="C8" s="73"/>
+      <c r="A8" s="66"/>
+      <c r="B8" s="73"/>
+      <c r="C8" s="74"/>
       <c r="D8" s="36" t="s">
         <v>120</v>
       </c>
@@ -2963,9 +3864,9 @@
       </c>
     </row>
     <row r="9" spans="1:11" ht="31.5">
-      <c r="A9" s="65"/>
-      <c r="B9" s="72"/>
-      <c r="C9" s="73"/>
+      <c r="A9" s="66"/>
+      <c r="B9" s="73"/>
+      <c r="C9" s="74"/>
       <c r="D9" s="35" t="s">
         <v>121</v>
       </c>
@@ -2992,9 +3893,9 @@
       </c>
     </row>
     <row r="10" spans="1:11" ht="31.5">
-      <c r="A10" s="66"/>
-      <c r="B10" s="74"/>
-      <c r="C10" s="75"/>
+      <c r="A10" s="67"/>
+      <c r="B10" s="75"/>
+      <c r="C10" s="76"/>
       <c r="D10" s="35" t="s">
         <v>122</v>
       </c>
@@ -3060,11 +3961,11 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:8">
-      <c r="F3" s="90" t="s">
+      <c r="F3" s="91" t="s">
         <v>40</v>
       </c>
-      <c r="G3" s="91"/>
-      <c r="H3" s="91"/>
+      <c r="G3" s="92"/>
+      <c r="H3" s="92"/>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" s="6" t="s">
@@ -3093,7 +3994,7 @@
       </c>
     </row>
     <row r="5" spans="1:8">
-      <c r="A5" s="88" t="s">
+      <c r="A5" s="89" t="s">
         <v>28</v>
       </c>
       <c r="B5" s="24" t="s">
@@ -3119,7 +4020,7 @@
       </c>
     </row>
     <row r="6" spans="1:8">
-      <c r="A6" s="88"/>
+      <c r="A6" s="89"/>
       <c r="B6" s="24" t="s">
         <v>151</v>
       </c>
@@ -3143,7 +4044,7 @@
       </c>
     </row>
     <row r="7" spans="1:8">
-      <c r="A7" s="88"/>
+      <c r="A7" s="89"/>
       <c r="B7" s="24" t="s">
         <v>25</v>
       </c>
@@ -3167,7 +4068,7 @@
       </c>
     </row>
     <row r="8" spans="1:8">
-      <c r="A8" s="88"/>
+      <c r="A8" s="89"/>
       <c r="B8" s="24" t="s">
         <v>27</v>
       </c>
@@ -3191,7 +4092,7 @@
       </c>
     </row>
     <row r="9" spans="1:8" ht="30">
-      <c r="A9" s="89" t="s">
+      <c r="A9" s="90" t="s">
         <v>152</v>
       </c>
       <c r="B9" s="24" t="s">
@@ -3213,7 +4114,7 @@
       <c r="H9" s="42"/>
     </row>
     <row r="10" spans="1:8">
-      <c r="A10" s="89"/>
+      <c r="A10" s="90"/>
       <c r="B10" s="24" t="s">
         <v>153</v>
       </c>
@@ -3233,7 +4134,7 @@
       <c r="H10" s="42"/>
     </row>
     <row r="11" spans="1:8">
-      <c r="A11" s="89"/>
+      <c r="A11" s="90"/>
       <c r="B11" s="24" t="s">
         <v>154</v>
       </c>
@@ -3253,7 +4154,7 @@
       <c r="H11" s="42"/>
     </row>
     <row r="12" spans="1:8">
-      <c r="A12" s="89"/>
+      <c r="A12" s="90"/>
       <c r="B12" s="24" t="s">
         <v>155</v>
       </c>
@@ -3273,7 +4174,7 @@
       <c r="H12" s="42"/>
     </row>
     <row r="13" spans="1:8">
-      <c r="A13" s="89"/>
+      <c r="A13" s="90"/>
       <c r="B13" s="25" t="s">
         <v>156</v>
       </c>
@@ -3304,10 +4205,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{129A480F-2285-4A8E-88CD-74850D6AFE43}">
-  <dimension ref="A1:N11"/>
+  <dimension ref="A1:Q11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="P8" sqref="P8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3322,32 +4223,37 @@
     <col min="14" max="14" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14">
+    <row r="1" spans="1:17">
       <c r="B1" s="38" t="s">
         <v>146</v>
       </c>
-      <c r="C1" s="92" t="s">
+      <c r="C1" s="93" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="93"/>
-      <c r="E1" s="94"/>
-      <c r="F1" s="92" t="s">
+      <c r="D1" s="94"/>
+      <c r="E1" s="95"/>
+      <c r="F1" s="93" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="93"/>
-      <c r="H1" s="94"/>
-      <c r="I1" s="92" t="s">
+      <c r="G1" s="94"/>
+      <c r="H1" s="95"/>
+      <c r="I1" s="93" t="s">
         <v>65</v>
       </c>
-      <c r="J1" s="93"/>
-      <c r="K1" s="94"/>
-      <c r="L1" s="95" t="s">
+      <c r="J1" s="94"/>
+      <c r="K1" s="95"/>
+      <c r="L1" s="96" t="s">
         <v>66</v>
       </c>
-      <c r="M1" s="96"/>
-      <c r="N1" s="96"/>
-    </row>
-    <row r="2" spans="1:14">
+      <c r="M1" s="97"/>
+      <c r="N1" s="97"/>
+      <c r="O1" s="93" t="s">
+        <v>131</v>
+      </c>
+      <c r="P1" s="94"/>
+      <c r="Q1" s="95"/>
+    </row>
+    <row r="2" spans="1:17">
       <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
@@ -3390,8 +4296,17 @@
       <c r="N2" s="37" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="3" spans="1:14">
+      <c r="O2" s="37" t="s">
+        <v>142</v>
+      </c>
+      <c r="P2" s="37" t="s">
+        <v>143</v>
+      </c>
+      <c r="Q2" s="37" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17">
       <c r="A3" s="23" t="s">
         <v>75</v>
       </c>
@@ -3438,8 +4353,18 @@
       <c r="N3" s="8" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="4" spans="1:14">
+      <c r="O3" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="P3" s="8" t="str">
+        <f>O3</f>
+        <v>V1.5</v>
+      </c>
+      <c r="Q3" s="8" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17">
       <c r="A4" s="23" t="s">
         <v>76</v>
       </c>
@@ -3486,8 +4411,18 @@
       <c r="N4" s="8" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="5" spans="1:14">
+      <c r="O4" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="P4" s="8" t="str">
+        <f t="shared" ref="P4" si="4">O4</f>
+        <v>V2.5</v>
+      </c>
+      <c r="Q4" s="8" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17">
       <c r="A5" s="39" t="s">
         <v>77</v>
       </c>
@@ -3514,8 +4449,13 @@
       <c r="N5" s="8" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="6" spans="1:14">
+      <c r="O5" s="8"/>
+      <c r="P5" s="8"/>
+      <c r="Q5" s="8" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17">
       <c r="A6" s="40" t="s">
         <v>78</v>
       </c>
@@ -3562,8 +4502,18 @@
       <c r="N6" s="8" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="11" spans="1:14">
+      <c r="O6" s="7">
+        <v>5.4</v>
+      </c>
+      <c r="P6" s="8">
+        <f t="shared" ref="P6" si="5">O6</f>
+        <v>5.4</v>
+      </c>
+      <c r="Q6" s="8" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17">
       <c r="B11" t="s">
         <v>87</v>
       </c>
@@ -3587,11 +4537,12 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="5">
     <mergeCell ref="C1:E1"/>
     <mergeCell ref="L1:N1"/>
     <mergeCell ref="I1:K1"/>
     <mergeCell ref="F1:H1"/>
+    <mergeCell ref="O1:Q1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3601,7 +4552,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9AD4D131-69ED-4813-926B-7E95E2B369DB}">
   <dimension ref="A1:N15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
@@ -3621,26 +4572,26 @@
       <c r="B1" s="38" t="s">
         <v>146</v>
       </c>
-      <c r="C1" s="92" t="s">
+      <c r="C1" s="93" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="93"/>
-      <c r="E1" s="94"/>
-      <c r="F1" s="92" t="s">
+      <c r="D1" s="94"/>
+      <c r="E1" s="95"/>
+      <c r="F1" s="93" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="93"/>
-      <c r="H1" s="94"/>
-      <c r="I1" s="92" t="s">
+      <c r="G1" s="94"/>
+      <c r="H1" s="95"/>
+      <c r="I1" s="93" t="s">
         <v>65</v>
       </c>
-      <c r="J1" s="93"/>
-      <c r="K1" s="94"/>
-      <c r="L1" s="95" t="s">
+      <c r="J1" s="94"/>
+      <c r="K1" s="95"/>
+      <c r="L1" s="96" t="s">
         <v>66</v>
       </c>
-      <c r="M1" s="96"/>
-      <c r="N1" s="96"/>
+      <c r="M1" s="97"/>
+      <c r="N1" s="97"/>
     </row>
     <row r="2" spans="1:14">
       <c r="A2" s="4" t="s">
@@ -3761,12 +4712,12 @@
       <c r="F5" s="8"/>
       <c r="G5" s="8"/>
       <c r="H5" s="8"/>
-      <c r="I5" s="97"/>
-      <c r="J5" s="97"/>
-      <c r="K5" s="97"/>
-      <c r="L5" s="97"/>
-      <c r="M5" s="97"/>
-      <c r="N5" s="97"/>
+      <c r="I5" s="43"/>
+      <c r="J5" s="43"/>
+      <c r="K5" s="43"/>
+      <c r="L5" s="43"/>
+      <c r="M5" s="43"/>
+      <c r="N5" s="43"/>
     </row>
     <row r="6" spans="1:14">
       <c r="A6" s="9" t="s">

</xml_diff>

<commit_message>
write match scenario - invoke matcher,fail test
</commit_message>
<xml_diff>
--- a/JavaExcelBDD/src/test/resources/ExcelBDD.xlsx
+++ b/JavaExcelBDD/src/test/resources/ExcelBDD.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/2fe8b90741a02718/Git/SimpleOpenExcelBDD/JavaExcelBDD/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="43" documentId="13_ncr:1_{2BC08F18-7250-451B-B716-B852607D4077}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6E37B364-7A12-4803-B6B2-14C59C4D0115}"/>
+  <xr:revisionPtr revIDLastSave="45" documentId="13_ncr:1_{2BC08F18-7250-451B-B716-B852607D4077}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D784D986-1BE9-456A-9FD1-5D2E1C54FAAF}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="9" xr2:uid="{965C72BA-AC7B-4020-96A1-B4855C2F0853}"/>
   </bookViews>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="620" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="620" uniqueCount="169">
   <si>
     <t>Role</t>
   </si>
@@ -549,6 +549,9 @@
   </si>
   <si>
     <t>V2.6</t>
+  </si>
+  <si>
+    <t>Scenario1b</t>
   </si>
 </sst>
 </file>
@@ -2045,8 +2048,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27202F44-224C-40C0-ACC3-02135A9560D7}">
   <dimension ref="A1:V11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="T7" sqref="T7"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="T2" sqref="T2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2093,7 +2096,7 @@
       <c r="R1" s="94"/>
       <c r="S1" s="95"/>
       <c r="T1" s="93" t="s">
-        <v>132</v>
+        <v>168</v>
       </c>
       <c r="U1" s="94"/>
       <c r="V1" s="95"/>

</xml_diff>

<commit_message>
add test on SBE matcher
</commit_message>
<xml_diff>
--- a/JavaExcelBDD/src/test/resources/ExcelBDD.xlsx
+++ b/JavaExcelBDD/src/test/resources/ExcelBDD.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/2fe8b90741a02718/Git/SimpleOpenExcelBDD/JavaExcelBDD/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="45" documentId="13_ncr:1_{2BC08F18-7250-451B-B716-B852607D4077}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D784D986-1BE9-456A-9FD1-5D2E1C54FAAF}"/>
+  <xr:revisionPtr revIDLastSave="55" documentId="13_ncr:1_{2BC08F18-7250-451B-B716-B852607D4077}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{99C28B43-8604-40E7-9B9A-C5C8F69C8097}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="9" xr2:uid="{965C72BA-AC7B-4020-96A1-B4855C2F0853}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{965C72BA-AC7B-4020-96A1-B4855C2F0853}"/>
   </bookViews>
   <sheets>
     <sheet name="SimpleOpenBDD" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="620" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="623" uniqueCount="171">
   <si>
     <t>Role</t>
   </si>
@@ -552,6 +552,12 @@
   </si>
   <si>
     <t>Scenario1b</t>
+  </si>
+  <si>
+    <t>Get count of test data set</t>
+  </si>
+  <si>
+    <t>TestDataSetCount</t>
   </si>
 </sst>
 </file>
@@ -859,7 +865,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="99">
+  <cellXfs count="96">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -890,9 +896,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="2" applyBorder="1"/>
@@ -950,15 +953,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
@@ -1114,6 +1108,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1627,10 +1624,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E1F2AA4-76D9-4C80-95B2-1FE7E77EF6CA}">
-  <dimension ref="A1:H17"/>
+  <dimension ref="A1:H18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:E17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1672,13 +1669,13 @@
       </c>
     </row>
     <row r="2" spans="1:8" ht="30">
-      <c r="A2" s="23">
+      <c r="A2" s="22">
         <v>1</v>
       </c>
-      <c r="B2" s="24" t="s">
+      <c r="B2" s="23" t="s">
         <v>28</v>
       </c>
-      <c r="C2" s="26" t="s">
+      <c r="C2" s="25" t="s">
         <v>29</v>
       </c>
       <c r="D2" s="6" t="s">
@@ -1698,13 +1695,13 @@
       </c>
     </row>
     <row r="3" spans="1:8">
-      <c r="A3" s="23">
+      <c r="A3" s="22">
         <v>2</v>
       </c>
-      <c r="B3" s="24" t="s">
+      <c r="B3" s="23" t="s">
         <v>25</v>
       </c>
-      <c r="C3" s="26" t="s">
+      <c r="C3" s="25" t="s">
         <v>29</v>
       </c>
       <c r="D3" s="6" t="s">
@@ -1724,13 +1721,13 @@
       </c>
     </row>
     <row r="4" spans="1:8" ht="30">
-      <c r="A4" s="23">
+      <c r="A4" s="22">
         <v>3</v>
       </c>
-      <c r="B4" s="24" t="s">
+      <c r="B4" s="23" t="s">
         <v>27</v>
       </c>
-      <c r="C4" s="26" t="s">
+      <c r="C4" s="25" t="s">
         <v>29</v>
       </c>
       <c r="D4" s="6" t="s">
@@ -1750,13 +1747,13 @@
       </c>
     </row>
     <row r="5" spans="1:8" ht="30">
-      <c r="A5" s="23">
+      <c r="A5" s="22">
         <v>4</v>
       </c>
-      <c r="B5" s="24" t="s">
+      <c r="B5" s="23" t="s">
         <v>31</v>
       </c>
-      <c r="C5" s="26" t="s">
+      <c r="C5" s="25" t="s">
         <v>5</v>
       </c>
       <c r="D5" s="6" t="s">
@@ -1776,13 +1773,13 @@
       </c>
     </row>
     <row r="6" spans="1:8">
-      <c r="A6" s="23">
+      <c r="A6" s="22">
         <v>5</v>
       </c>
-      <c r="B6" s="24" t="s">
+      <c r="B6" s="23" t="s">
         <v>32</v>
       </c>
-      <c r="C6" s="26" t="s">
+      <c r="C6" s="25" t="s">
         <v>5</v>
       </c>
       <c r="D6" s="6" t="s">
@@ -1802,13 +1799,13 @@
       </c>
     </row>
     <row r="7" spans="1:8">
-      <c r="A7" s="23">
+      <c r="A7" s="22">
         <v>6</v>
       </c>
-      <c r="B7" s="24" t="s">
+      <c r="B7" s="23" t="s">
         <v>35</v>
       </c>
-      <c r="C7" s="26" t="s">
+      <c r="C7" s="25" t="s">
         <v>5</v>
       </c>
       <c r="D7" s="6" t="s">
@@ -1828,13 +1825,13 @@
       </c>
     </row>
     <row r="8" spans="1:8" ht="30">
-      <c r="A8" s="23">
+      <c r="A8" s="22">
         <v>7</v>
       </c>
-      <c r="B8" s="25" t="s">
+      <c r="B8" s="24" t="s">
         <v>69</v>
       </c>
-      <c r="C8" s="26" t="s">
+      <c r="C8" s="25" t="s">
         <v>5</v>
       </c>
       <c r="D8" s="6" t="s">
@@ -1854,13 +1851,13 @@
       </c>
     </row>
     <row r="9" spans="1:8" ht="30">
-      <c r="A9" s="23">
+      <c r="A9" s="22">
         <v>8</v>
       </c>
-      <c r="B9" s="25" t="s">
+      <c r="B9" s="24" t="s">
         <v>70</v>
       </c>
-      <c r="C9" s="26" t="s">
+      <c r="C9" s="25" t="s">
         <v>5</v>
       </c>
       <c r="D9" s="6" t="s">
@@ -1880,13 +1877,13 @@
       </c>
     </row>
     <row r="10" spans="1:8">
-      <c r="A10" s="23">
+      <c r="A10" s="22">
         <v>9</v>
       </c>
-      <c r="B10" s="25" t="s">
+      <c r="B10" s="24" t="s">
         <v>67</v>
       </c>
-      <c r="C10" s="26" t="s">
+      <c r="C10" s="25" t="s">
         <v>5</v>
       </c>
       <c r="D10" s="6" t="s">
@@ -1898,13 +1895,13 @@
       <c r="H10" s="7"/>
     </row>
     <row r="11" spans="1:8" ht="30">
-      <c r="A11" s="23">
+      <c r="A11" s="22">
         <v>10</v>
       </c>
-      <c r="B11" s="24" t="s">
+      <c r="B11" s="23" t="s">
         <v>82</v>
       </c>
-      <c r="C11" s="26" t="s">
+      <c r="C11" s="25" t="s">
         <v>5</v>
       </c>
       <c r="D11" s="6" t="s">
@@ -1916,101 +1913,101 @@
       <c r="H11" s="7"/>
     </row>
     <row r="12" spans="1:8" ht="45">
-      <c r="A12" s="47">
+      <c r="A12" s="43">
         <v>11</v>
       </c>
-      <c r="B12" s="24" t="s">
+      <c r="B12" s="23" t="s">
         <v>89</v>
       </c>
-      <c r="C12" s="50" t="s">
+      <c r="C12" s="46" t="s">
         <v>5</v>
       </c>
-      <c r="D12" s="51" t="s">
+      <c r="D12" s="47" t="s">
         <v>86</v>
       </c>
-      <c r="E12" s="44">
+      <c r="E12" s="7">
         <v>3</v>
       </c>
-      <c r="F12" s="44">
+      <c r="F12" s="7">
         <v>3</v>
       </c>
-      <c r="G12" s="44">
+      <c r="G12" s="7">
         <v>3</v>
       </c>
-      <c r="H12" s="44">
+      <c r="H12" s="7">
         <v>3</v>
       </c>
     </row>
     <row r="13" spans="1:8">
-      <c r="A13" s="48"/>
-      <c r="B13" s="21" t="s">
+      <c r="A13" s="44"/>
+      <c r="B13" s="20" t="s">
         <v>97</v>
       </c>
-      <c r="C13" s="50"/>
-      <c r="D13" s="52"/>
-      <c r="E13" s="45"/>
-      <c r="F13" s="45"/>
-      <c r="G13" s="45"/>
-      <c r="H13" s="45"/>
+      <c r="C13" s="46"/>
+      <c r="D13" s="48"/>
+      <c r="E13" s="7"/>
+      <c r="F13" s="7"/>
+      <c r="G13" s="7"/>
+      <c r="H13" s="7"/>
     </row>
     <row r="14" spans="1:8">
-      <c r="A14" s="48"/>
-      <c r="B14" s="21" t="s">
+      <c r="A14" s="44"/>
+      <c r="B14" s="20" t="s">
         <v>84</v>
       </c>
-      <c r="C14" s="50"/>
-      <c r="D14" s="52"/>
-      <c r="E14" s="45"/>
-      <c r="F14" s="45"/>
-      <c r="G14" s="45"/>
-      <c r="H14" s="45"/>
+      <c r="C14" s="46"/>
+      <c r="D14" s="48"/>
+      <c r="E14" s="7"/>
+      <c r="F14" s="7"/>
+      <c r="G14" s="7"/>
+      <c r="H14" s="7"/>
     </row>
     <row r="15" spans="1:8">
-      <c r="A15" s="49"/>
-      <c r="B15" s="22" t="s">
+      <c r="A15" s="45"/>
+      <c r="B15" s="21" t="s">
         <v>85</v>
       </c>
-      <c r="C15" s="50"/>
-      <c r="D15" s="53"/>
-      <c r="E15" s="46"/>
-      <c r="F15" s="46"/>
-      <c r="G15" s="46"/>
-      <c r="H15" s="46"/>
+      <c r="C15" s="46"/>
+      <c r="D15" s="49"/>
+      <c r="E15" s="7"/>
+      <c r="F15" s="7"/>
+      <c r="G15" s="7"/>
+      <c r="H15" s="7"/>
     </row>
     <row r="16" spans="1:8" ht="30">
-      <c r="A16" s="26">
+      <c r="A16" s="25">
         <v>12</v>
       </c>
-      <c r="B16" s="27" t="s">
+      <c r="B16" s="26" t="s">
         <v>90</v>
       </c>
-      <c r="C16" s="26" t="s">
+      <c r="C16" s="25" t="s">
         <v>5</v>
       </c>
       <c r="D16" s="16" t="s">
         <v>96</v>
       </c>
-      <c r="E16" s="17" t="s">
+      <c r="E16" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="F16" s="17" t="s">
+      <c r="F16" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="G16" s="17" t="s">
+      <c r="G16" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="H16" s="17" t="s">
+      <c r="H16" s="7" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="30">
-      <c r="A17" s="26">
+      <c r="A17" s="25">
         <v>13</v>
       </c>
-      <c r="B17" s="27" t="s">
+      <c r="B17" s="26" t="s">
         <v>37</v>
       </c>
-      <c r="C17" s="26" t="s">
+      <c r="C17" s="25" t="s">
         <v>5</v>
       </c>
       <c r="D17" s="6" t="s">
@@ -2029,15 +2026,37 @@
         <v>5</v>
       </c>
     </row>
+    <row r="18" spans="1:8">
+      <c r="A18" s="2">
+        <v>14</v>
+      </c>
+      <c r="B18" s="95" t="s">
+        <v>169</v>
+      </c>
+      <c r="C18" s="25" t="s">
+        <v>5</v>
+      </c>
+      <c r="D18" s="6" t="s">
+        <v>170</v>
+      </c>
+      <c r="E18" s="7">
+        <v>4</v>
+      </c>
+      <c r="F18" s="7">
+        <v>4</v>
+      </c>
+      <c r="G18" s="7">
+        <v>4</v>
+      </c>
+      <c r="H18" s="7">
+        <v>4</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="7">
-    <mergeCell ref="H12:H15"/>
+  <mergeCells count="3">
     <mergeCell ref="A12:A15"/>
     <mergeCell ref="C12:C15"/>
     <mergeCell ref="D12:D15"/>
-    <mergeCell ref="E12:E15"/>
-    <mergeCell ref="F12:F15"/>
-    <mergeCell ref="G12:G15"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2048,7 +2067,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27202F44-224C-40C0-ACC3-02135A9560D7}">
   <dimension ref="A1:V11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+    <sheetView topLeftCell="C1" workbookViewId="0">
       <selection activeCell="T2" sqref="T2"/>
     </sheetView>
   </sheetViews>
@@ -2067,39 +2086,39 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22">
-      <c r="D1" s="38" t="s">
+      <c r="D1" s="37" t="s">
         <v>146</v>
       </c>
-      <c r="E1" s="93" t="s">
+      <c r="E1" s="89" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="94"/>
-      <c r="G1" s="95"/>
-      <c r="H1" s="93" t="s">
+      <c r="F1" s="90"/>
+      <c r="G1" s="91"/>
+      <c r="H1" s="89" t="s">
         <v>4</v>
       </c>
-      <c r="I1" s="94"/>
-      <c r="J1" s="95"/>
-      <c r="K1" s="93" t="s">
+      <c r="I1" s="90"/>
+      <c r="J1" s="91"/>
+      <c r="K1" s="89" t="s">
         <v>65</v>
       </c>
-      <c r="L1" s="94"/>
-      <c r="M1" s="95"/>
-      <c r="N1" s="98" t="s">
+      <c r="L1" s="90"/>
+      <c r="M1" s="91"/>
+      <c r="N1" s="94" t="s">
         <v>66</v>
       </c>
-      <c r="O1" s="98"/>
-      <c r="P1" s="98"/>
-      <c r="Q1" s="93" t="s">
+      <c r="O1" s="94"/>
+      <c r="P1" s="94"/>
+      <c r="Q1" s="89" t="s">
         <v>131</v>
       </c>
-      <c r="R1" s="94"/>
-      <c r="S1" s="95"/>
-      <c r="T1" s="93" t="s">
+      <c r="R1" s="90"/>
+      <c r="S1" s="91"/>
+      <c r="T1" s="89" t="s">
         <v>168</v>
       </c>
-      <c r="U1" s="94"/>
-      <c r="V1" s="95"/>
+      <c r="U1" s="90"/>
+      <c r="V1" s="91"/>
     </row>
     <row r="2" spans="1:22">
       <c r="A2" s="4" t="s">
@@ -2114,58 +2133,58 @@
       <c r="D2" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="E2" s="37" t="s">
+      <c r="E2" s="36" t="s">
         <v>142</v>
       </c>
-      <c r="F2" s="37" t="s">
+      <c r="F2" s="36" t="s">
         <v>143</v>
       </c>
-      <c r="G2" s="37" t="s">
+      <c r="G2" s="36" t="s">
         <v>144</v>
       </c>
-      <c r="H2" s="37" t="s">
+      <c r="H2" s="36" t="s">
         <v>142</v>
       </c>
-      <c r="I2" s="37" t="s">
+      <c r="I2" s="36" t="s">
         <v>143</v>
       </c>
-      <c r="J2" s="37" t="s">
+      <c r="J2" s="36" t="s">
         <v>144</v>
       </c>
-      <c r="K2" s="37" t="s">
+      <c r="K2" s="36" t="s">
         <v>142</v>
       </c>
-      <c r="L2" s="37" t="s">
+      <c r="L2" s="36" t="s">
         <v>143</v>
       </c>
-      <c r="M2" s="37" t="s">
+      <c r="M2" s="36" t="s">
         <v>144</v>
       </c>
-      <c r="N2" s="37" t="s">
+      <c r="N2" s="36" t="s">
         <v>142</v>
       </c>
-      <c r="O2" s="37" t="s">
+      <c r="O2" s="36" t="s">
         <v>143</v>
       </c>
-      <c r="P2" s="37" t="s">
+      <c r="P2" s="36" t="s">
         <v>144</v>
       </c>
-      <c r="Q2" s="37" t="s">
+      <c r="Q2" s="36" t="s">
         <v>142</v>
       </c>
-      <c r="R2" s="37" t="s">
+      <c r="R2" s="36" t="s">
         <v>143</v>
       </c>
-      <c r="S2" s="37" t="s">
+      <c r="S2" s="36" t="s">
         <v>144</v>
       </c>
-      <c r="T2" s="37" t="s">
+      <c r="T2" s="36" t="s">
         <v>142</v>
       </c>
-      <c r="U2" s="37" t="s">
+      <c r="U2" s="36" t="s">
         <v>143</v>
       </c>
-      <c r="V2" s="37" t="s">
+      <c r="V2" s="36" t="s">
         <v>144</v>
       </c>
     </row>
@@ -2173,10 +2192,10 @@
       <c r="A3" s="9">
         <v>1</v>
       </c>
-      <c r="B3" s="23" t="s">
+      <c r="B3" s="22" t="s">
         <v>75</v>
       </c>
-      <c r="C3" s="23"/>
+      <c r="C3" s="22"/>
       <c r="D3" s="4" t="s">
         <v>13</v>
       </c>
@@ -2245,10 +2264,10 @@
       <c r="A4" s="9">
         <v>2</v>
       </c>
-      <c r="B4" s="23" t="s">
+      <c r="B4" s="22" t="s">
         <v>76</v>
       </c>
-      <c r="C4" s="23"/>
+      <c r="C4" s="22"/>
       <c r="D4" s="4" t="s">
         <v>14</v>
       </c>
@@ -2317,10 +2336,10 @@
       <c r="A5" s="9">
         <v>3</v>
       </c>
-      <c r="B5" s="39" t="s">
+      <c r="B5" s="38" t="s">
         <v>77</v>
       </c>
-      <c r="C5" s="39"/>
+      <c r="C5" s="38"/>
       <c r="D5" s="4" t="s">
         <v>15</v>
       </c>
@@ -2359,14 +2378,14 @@
       <c r="A6" s="9">
         <v>4</v>
       </c>
-      <c r="B6" s="40" t="s">
+      <c r="B6" s="39" t="s">
         <v>78</v>
       </c>
-      <c r="C6" s="40"/>
+      <c r="C6" s="39"/>
       <c r="D6" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="E6" s="30" t="s">
+      <c r="E6" s="29" t="s">
         <v>100</v>
       </c>
       <c r="F6" s="8" t="str">
@@ -2386,7 +2405,7 @@
       <c r="J6" s="8" t="s">
         <v>145</v>
       </c>
-      <c r="K6" s="29" t="b">
+      <c r="K6" s="28" t="b">
         <v>1</v>
       </c>
       <c r="L6" s="8" t="b">
@@ -2486,34 +2505,34 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:19">
-      <c r="D3" s="38" t="s">
+      <c r="D3" s="37" t="s">
         <v>146</v>
       </c>
-      <c r="E3" s="93" t="s">
+      <c r="E3" s="89" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="94"/>
-      <c r="G3" s="95"/>
-      <c r="H3" s="93" t="s">
+      <c r="F3" s="90"/>
+      <c r="G3" s="91"/>
+      <c r="H3" s="89" t="s">
         <v>4</v>
       </c>
-      <c r="I3" s="94"/>
-      <c r="J3" s="95"/>
-      <c r="K3" s="93" t="s">
+      <c r="I3" s="90"/>
+      <c r="J3" s="91"/>
+      <c r="K3" s="89" t="s">
         <v>65</v>
       </c>
-      <c r="L3" s="94"/>
-      <c r="M3" s="95"/>
-      <c r="N3" s="98" t="s">
+      <c r="L3" s="90"/>
+      <c r="M3" s="91"/>
+      <c r="N3" s="94" t="s">
         <v>66</v>
       </c>
-      <c r="O3" s="98"/>
-      <c r="P3" s="98"/>
-      <c r="Q3" s="93" t="s">
+      <c r="O3" s="94"/>
+      <c r="P3" s="94"/>
+      <c r="Q3" s="89" t="s">
         <v>131</v>
       </c>
-      <c r="R3" s="94"/>
-      <c r="S3" s="95"/>
+      <c r="R3" s="90"/>
+      <c r="S3" s="91"/>
     </row>
     <row r="4" spans="1:19">
       <c r="A4" s="4" t="s">
@@ -2528,49 +2547,49 @@
       <c r="D4" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="E4" s="37" t="s">
+      <c r="E4" s="36" t="s">
         <v>142</v>
       </c>
-      <c r="F4" s="37" t="s">
+      <c r="F4" s="36" t="s">
         <v>143</v>
       </c>
-      <c r="G4" s="37" t="s">
+      <c r="G4" s="36" t="s">
         <v>144</v>
       </c>
-      <c r="H4" s="37" t="s">
+      <c r="H4" s="36" t="s">
         <v>142</v>
       </c>
-      <c r="I4" s="37" t="s">
+      <c r="I4" s="36" t="s">
         <v>143</v>
       </c>
-      <c r="J4" s="37" t="s">
+      <c r="J4" s="36" t="s">
         <v>144</v>
       </c>
-      <c r="K4" s="37" t="s">
+      <c r="K4" s="36" t="s">
         <v>142</v>
       </c>
-      <c r="L4" s="37" t="s">
+      <c r="L4" s="36" t="s">
         <v>143</v>
       </c>
-      <c r="M4" s="37" t="s">
+      <c r="M4" s="36" t="s">
         <v>144</v>
       </c>
-      <c r="N4" s="37" t="s">
+      <c r="N4" s="36" t="s">
         <v>142</v>
       </c>
-      <c r="O4" s="37" t="s">
+      <c r="O4" s="36" t="s">
         <v>143</v>
       </c>
-      <c r="P4" s="37" t="s">
+      <c r="P4" s="36" t="s">
         <v>144</v>
       </c>
-      <c r="Q4" s="37" t="s">
+      <c r="Q4" s="36" t="s">
         <v>142</v>
       </c>
-      <c r="R4" s="37" t="s">
+      <c r="R4" s="36" t="s">
         <v>143</v>
       </c>
-      <c r="S4" s="37" t="s">
+      <c r="S4" s="36" t="s">
         <v>144</v>
       </c>
     </row>
@@ -2578,10 +2597,10 @@
       <c r="A5" s="9">
         <v>1</v>
       </c>
-      <c r="B5" s="23" t="s">
+      <c r="B5" s="22" t="s">
         <v>75</v>
       </c>
-      <c r="C5" s="23"/>
+      <c r="C5" s="22"/>
       <c r="D5" s="4" t="s">
         <v>13</v>
       </c>
@@ -2640,10 +2659,10 @@
       <c r="A6" s="9">
         <v>2</v>
       </c>
-      <c r="B6" s="23" t="s">
+      <c r="B6" s="22" t="s">
         <v>76</v>
       </c>
-      <c r="C6" s="23"/>
+      <c r="C6" s="22"/>
       <c r="D6" s="4" t="s">
         <v>14</v>
       </c>
@@ -2702,10 +2721,10 @@
       <c r="A7" s="9">
         <v>3</v>
       </c>
-      <c r="B7" s="39" t="s">
+      <c r="B7" s="38" t="s">
         <v>77</v>
       </c>
-      <c r="C7" s="39"/>
+      <c r="C7" s="38"/>
       <c r="D7" s="4" t="s">
         <v>15</v>
       </c>
@@ -2739,14 +2758,14 @@
       <c r="A8" s="9">
         <v>4</v>
       </c>
-      <c r="B8" s="40" t="s">
+      <c r="B8" s="39" t="s">
         <v>78</v>
       </c>
-      <c r="C8" s="40"/>
+      <c r="C8" s="39"/>
       <c r="D8" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="E8" s="30" t="s">
+      <c r="E8" s="29" t="s">
         <v>100</v>
       </c>
       <c r="F8" s="8" t="str">
@@ -2766,7 +2785,7 @@
       <c r="J8" s="8" t="s">
         <v>145</v>
       </c>
-      <c r="K8" s="29" t="b">
+      <c r="K8" s="28" t="b">
         <v>1</v>
       </c>
       <c r="L8" s="8" t="b">
@@ -2868,7 +2887,7 @@
       <c r="F1" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="G1" s="20" t="s">
+      <c r="G1" s="19" t="s">
         <v>92</v>
       </c>
     </row>
@@ -2891,7 +2910,7 @@
       <c r="F2" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="G2" s="19" t="s">
+      <c r="G2" s="18" t="s">
         <v>93</v>
       </c>
     </row>
@@ -2914,39 +2933,39 @@
       <c r="F3" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="G3" s="19" t="s">
+      <c r="G3" s="18" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="4" spans="1:7">
-      <c r="A4" s="18"/>
+      <c r="A4" s="17"/>
       <c r="B4" s="4"/>
       <c r="C4" s="8"/>
       <c r="D4" s="8"/>
       <c r="E4" s="8"/>
       <c r="F4" s="8"/>
-      <c r="G4" s="19"/>
+      <c r="G4" s="18"/>
     </row>
     <row r="5" spans="1:7">
-      <c r="A5" s="18"/>
+      <c r="A5" s="17"/>
       <c r="B5" s="4"/>
       <c r="C5" s="8"/>
       <c r="D5" s="8"/>
       <c r="E5" s="8"/>
       <c r="F5" s="8"/>
-      <c r="G5" s="19"/>
+      <c r="G5" s="18"/>
     </row>
     <row r="6" spans="1:7">
-      <c r="A6" s="18"/>
+      <c r="A6" s="17"/>
       <c r="B6" s="4"/>
       <c r="C6" s="8"/>
       <c r="D6" s="8"/>
       <c r="E6" s="8"/>
       <c r="F6" s="8"/>
-      <c r="G6" s="19"/>
+      <c r="G6" s="18"/>
     </row>
     <row r="7" spans="1:7">
-      <c r="A7" s="54" t="s">
+      <c r="A7" s="50" t="s">
         <v>77</v>
       </c>
       <c r="B7" s="4" t="s">
@@ -2956,10 +2975,10 @@
       <c r="D7" s="8"/>
       <c r="E7" s="8"/>
       <c r="F7" s="8"/>
-      <c r="G7" s="19"/>
+      <c r="G7" s="18"/>
     </row>
     <row r="8" spans="1:7">
-      <c r="A8" s="55"/>
+      <c r="A8" s="51"/>
       <c r="B8" s="4" t="s">
         <v>83</v>
       </c>
@@ -2967,33 +2986,33 @@
       <c r="D8" s="8"/>
       <c r="E8" s="8"/>
       <c r="F8" s="8"/>
-      <c r="G8" s="19"/>
+      <c r="G8" s="18"/>
     </row>
     <row r="9" spans="1:7">
-      <c r="A9" s="56" t="s">
+      <c r="A9" s="52" t="s">
         <v>78</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C9" s="30" t="s">
+      <c r="C9" s="29" t="s">
         <v>100</v>
       </c>
       <c r="D9" s="8" t="b">
         <v>0</v>
       </c>
-      <c r="E9" s="29" t="b">
+      <c r="E9" s="28" t="b">
         <v>1</v>
       </c>
       <c r="F9" s="7">
         <v>4.4000000000000004</v>
       </c>
-      <c r="G9" s="19" t="s">
+      <c r="G9" s="18" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="10" spans="1:7">
-      <c r="A10" s="57"/>
+      <c r="A10" s="53"/>
       <c r="B10" s="15" t="s">
         <v>83</v>
       </c>
@@ -3001,7 +3020,7 @@
       <c r="D10" s="8"/>
       <c r="E10" s="8"/>
       <c r="F10" s="8"/>
-      <c r="G10" s="19"/>
+      <c r="G10" s="18"/>
     </row>
     <row r="15" spans="1:7">
       <c r="B15" t="s">
@@ -3067,7 +3086,7 @@
       <c r="E1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="20" t="s">
+      <c r="F1" s="19" t="s">
         <v>92</v>
       </c>
       <c r="G1" s="5" t="s">
@@ -3083,7 +3102,7 @@
       <c r="C2" s="5"/>
       <c r="D2" s="5"/>
       <c r="E2" s="5"/>
-      <c r="F2" s="19"/>
+      <c r="F2" s="18"/>
       <c r="G2" s="5"/>
       <c r="H2" s="5"/>
     </row>
@@ -3103,7 +3122,7 @@
       <c r="E3" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="F3" s="19" t="s">
+      <c r="F3" s="18" t="s">
         <v>93</v>
       </c>
       <c r="G3" s="8" t="s">
@@ -3121,7 +3140,7 @@
       </c>
       <c r="D4" s="8"/>
       <c r="E4" s="8"/>
-      <c r="F4" s="19"/>
+      <c r="F4" s="18"/>
       <c r="G4" s="8"/>
       <c r="H4" s="8"/>
     </row>
@@ -3133,7 +3152,7 @@
       <c r="C5" s="4"/>
       <c r="D5" s="8"/>
       <c r="E5" s="8"/>
-      <c r="F5" s="19"/>
+      <c r="F5" s="18"/>
       <c r="G5" s="8"/>
       <c r="H5" s="8"/>
     </row>
@@ -3143,7 +3162,7 @@
       <c r="C6" s="4"/>
       <c r="D6" s="8"/>
       <c r="E6" s="8"/>
-      <c r="F6" s="19"/>
+      <c r="F6" s="18"/>
       <c r="G6" s="8"/>
       <c r="H6" s="8"/>
     </row>
@@ -3164,7 +3183,7 @@
         <f>E14</f>
         <v>V2.2</v>
       </c>
-      <c r="F7" s="19" t="s">
+      <c r="F7" s="18" t="s">
         <v>94</v>
       </c>
       <c r="G7" s="8" t="s">
@@ -3186,7 +3205,7 @@
       </c>
       <c r="D8" s="8"/>
       <c r="E8" s="8"/>
-      <c r="F8" s="19"/>
+      <c r="F8" s="18"/>
       <c r="G8" s="8"/>
       <c r="H8" s="8"/>
     </row>
@@ -3200,16 +3219,16 @@
       <c r="C9" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="D9" s="30" t="s">
+      <c r="D9" s="29" t="s">
         <v>100</v>
       </c>
       <c r="E9" s="8" t="b">
         <v>0</v>
       </c>
-      <c r="F9" s="19" t="s">
+      <c r="F9" s="18" t="s">
         <v>95</v>
       </c>
-      <c r="G9" s="29" t="b">
+      <c r="G9" s="28" t="b">
         <v>1</v>
       </c>
       <c r="H9" s="7">
@@ -3217,7 +3236,7 @@
       </c>
     </row>
     <row r="12" spans="1:8">
-      <c r="A12" s="28" t="s">
+      <c r="A12" s="27" t="s">
         <v>99</v>
       </c>
     </row>
@@ -3265,15 +3284,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="58" t="s">
+      <c r="A1" s="54" t="s">
         <v>43</v>
       </c>
-      <c r="B1" s="58"/>
-      <c r="C1" s="58"/>
-      <c r="D1" s="58"/>
-      <c r="E1" s="58"/>
-      <c r="F1" s="58"/>
-      <c r="G1" s="58"/>
+      <c r="B1" s="54"/>
+      <c r="C1" s="54"/>
+      <c r="D1" s="54"/>
+      <c r="E1" s="54"/>
+      <c r="F1" s="54"/>
+      <c r="G1" s="54"/>
       <c r="H1" s="2"/>
     </row>
     <row r="2" spans="1:8">
@@ -3309,7 +3328,7 @@
       <c r="B3" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="C3" s="59" t="s">
+      <c r="C3" s="55" t="s">
         <v>46</v>
       </c>
       <c r="D3" s="4" t="s">
@@ -3335,7 +3354,7 @@
       <c r="B4" s="9" t="s">
         <v>76</v>
       </c>
-      <c r="C4" s="60"/>
+      <c r="C4" s="56"/>
       <c r="D4" s="4" t="s">
         <v>14</v>
       </c>
@@ -3359,7 +3378,7 @@
       <c r="B5" s="9" t="s">
         <v>77</v>
       </c>
-      <c r="C5" s="61"/>
+      <c r="C5" s="57"/>
       <c r="D5" s="4" t="s">
         <v>15</v>
       </c>
@@ -3379,13 +3398,13 @@
       <c r="D6" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="E6" s="30" t="s">
+      <c r="E6" s="29" t="s">
         <v>100</v>
       </c>
       <c r="F6" s="8" t="b">
         <v>0</v>
       </c>
-      <c r="G6" s="29" t="b">
+      <c r="G6" s="28" t="b">
         <v>1</v>
       </c>
       <c r="H6" s="7">
@@ -3437,42 +3456,42 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
-      <c r="A1" s="64" t="s">
+      <c r="A1" s="60" t="s">
         <v>50</v>
       </c>
-      <c r="B1" s="64"/>
-      <c r="C1" s="58" t="s">
+      <c r="B1" s="60"/>
+      <c r="C1" s="54" t="s">
         <v>64</v>
       </c>
-      <c r="D1" s="58"/>
+      <c r="D1" s="54"/>
       <c r="E1" s="14" t="s">
         <v>51</v>
       </c>
-      <c r="F1" s="62" t="s">
+      <c r="F1" s="58" t="s">
         <v>52</v>
       </c>
-      <c r="G1" s="63"/>
-      <c r="H1" s="63"/>
-      <c r="I1" s="63"/>
+      <c r="G1" s="59"/>
+      <c r="H1" s="59"/>
+      <c r="I1" s="59"/>
     </row>
     <row r="2" spans="1:9">
-      <c r="A2" s="64" t="s">
+      <c r="A2" s="60" t="s">
         <v>53</v>
       </c>
-      <c r="B2" s="64"/>
-      <c r="C2" s="70" t="s">
+      <c r="B2" s="60"/>
+      <c r="C2" s="66" t="s">
         <v>49</v>
       </c>
-      <c r="D2" s="70"/>
+      <c r="D2" s="66"/>
       <c r="E2" s="11" t="s">
         <v>80</v>
       </c>
-      <c r="F2" s="68" t="s">
+      <c r="F2" s="64" t="s">
         <v>81</v>
       </c>
-      <c r="G2" s="68"/>
-      <c r="H2" s="68"/>
-      <c r="I2" s="69"/>
+      <c r="G2" s="64"/>
+      <c r="H2" s="64"/>
+      <c r="I2" s="65"/>
     </row>
     <row r="3" spans="1:9">
       <c r="A3" s="13" t="s">
@@ -3504,16 +3523,16 @@
       </c>
     </row>
     <row r="4" spans="1:9" ht="69.95" customHeight="1">
-      <c r="A4" s="65" t="s">
+      <c r="A4" s="61" t="s">
         <v>57</v>
       </c>
       <c r="B4" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="C4" s="65" t="s">
+      <c r="C4" s="61" t="s">
         <v>48</v>
       </c>
-      <c r="D4" s="59" t="s">
+      <c r="D4" s="55" t="s">
         <v>46</v>
       </c>
       <c r="E4" s="4" t="s">
@@ -3533,12 +3552,12 @@
       </c>
     </row>
     <row r="5" spans="1:9" ht="69.95" customHeight="1">
-      <c r="A5" s="66"/>
+      <c r="A5" s="62"/>
       <c r="B5" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="C5" s="66"/>
-      <c r="D5" s="60"/>
+      <c r="C5" s="62"/>
+      <c r="D5" s="56"/>
       <c r="E5" s="4" t="s">
         <v>14</v>
       </c>
@@ -3556,12 +3575,12 @@
       </c>
     </row>
     <row r="6" spans="1:9" ht="69.95" customHeight="1">
-      <c r="A6" s="66"/>
+      <c r="A6" s="62"/>
       <c r="B6" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="C6" s="67"/>
-      <c r="D6" s="61"/>
+      <c r="C6" s="63"/>
+      <c r="D6" s="57"/>
       <c r="E6" s="4" t="s">
         <v>15</v>
       </c>
@@ -3571,7 +3590,7 @@
       <c r="I6" s="8"/>
     </row>
     <row r="7" spans="1:9">
-      <c r="A7" s="67"/>
+      <c r="A7" s="63"/>
       <c r="B7" s="9" t="s">
         <v>61</v>
       </c>
@@ -3584,13 +3603,13 @@
       <c r="E7" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="F7" s="30" t="s">
+      <c r="F7" s="29" t="s">
         <v>100</v>
       </c>
       <c r="G7" s="8" t="b">
         <v>0</v>
       </c>
-      <c r="H7" s="29" t="b">
+      <c r="H7" s="28" t="b">
         <v>1</v>
       </c>
       <c r="I7" s="7">
@@ -3655,41 +3674,41 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="23.25">
-      <c r="A1" s="64" t="s">
+      <c r="A1" s="60" t="s">
         <v>50</v>
       </c>
-      <c r="B1" s="64"/>
-      <c r="C1" s="83" t="s">
+      <c r="B1" s="60"/>
+      <c r="C1" s="79" t="s">
         <v>101</v>
       </c>
-      <c r="D1" s="83"/>
-      <c r="E1" s="83"/>
-      <c r="F1" s="83"/>
-      <c r="G1" s="83"/>
-      <c r="H1" s="83"/>
+      <c r="D1" s="79"/>
+      <c r="E1" s="79"/>
+      <c r="F1" s="79"/>
+      <c r="G1" s="79"/>
+      <c r="H1" s="79"/>
     </row>
     <row r="2" spans="1:11" ht="38.25" customHeight="1">
-      <c r="A2" s="88" t="s">
+      <c r="A2" s="84" t="s">
         <v>53</v>
       </c>
-      <c r="B2" s="88"/>
-      <c r="C2" s="84" t="s">
+      <c r="B2" s="84"/>
+      <c r="C2" s="80" t="s">
         <v>102</v>
       </c>
-      <c r="D2" s="84"/>
-      <c r="E2" s="84"/>
-      <c r="F2" s="84"/>
-      <c r="G2" s="84"/>
-      <c r="H2" s="84"/>
+      <c r="D2" s="80"/>
+      <c r="E2" s="80"/>
+      <c r="F2" s="80"/>
+      <c r="G2" s="80"/>
+      <c r="H2" s="80"/>
     </row>
     <row r="3" spans="1:11">
       <c r="A3" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="85" t="s">
+      <c r="B3" s="81" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="86"/>
+      <c r="C3" s="82"/>
       <c r="D3" s="13" t="s">
         <v>111</v>
       </c>
@@ -3716,211 +3735,211 @@
       </c>
     </row>
     <row r="4" spans="1:11" ht="15" customHeight="1">
-      <c r="A4" s="65" t="s">
+      <c r="A4" s="61" t="s">
         <v>57</v>
       </c>
-      <c r="B4" s="77" t="s">
+      <c r="B4" s="73" t="s">
         <v>104</v>
       </c>
-      <c r="C4" s="78"/>
-      <c r="D4" s="79"/>
-      <c r="E4" s="31" t="s">
+      <c r="C4" s="74"/>
+      <c r="D4" s="75"/>
+      <c r="E4" s="30" t="s">
         <v>103</v>
       </c>
-      <c r="F4" s="32" t="s">
+      <c r="F4" s="31" t="s">
         <v>105</v>
       </c>
-      <c r="G4" s="32" t="s">
+      <c r="G4" s="31" t="s">
         <v>105</v>
       </c>
-      <c r="H4" s="32" t="s">
+      <c r="H4" s="31" t="s">
         <v>105</v>
       </c>
-      <c r="I4" s="32" t="s">
+      <c r="I4" s="31" t="s">
         <v>133</v>
       </c>
-      <c r="J4" s="32" t="s">
+      <c r="J4" s="31" t="s">
         <v>134</v>
       </c>
-      <c r="K4" s="32" t="s">
+      <c r="K4" s="31" t="s">
         <v>135</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="51.75" customHeight="1">
-      <c r="A5" s="66"/>
-      <c r="B5" s="87" t="s">
+      <c r="A5" s="62"/>
+      <c r="B5" s="83" t="s">
         <v>107</v>
       </c>
-      <c r="C5" s="87"/>
-      <c r="D5" s="35" t="s">
+      <c r="C5" s="83"/>
+      <c r="D5" s="34" t="s">
         <v>113</v>
       </c>
-      <c r="E5" s="31" t="s">
+      <c r="E5" s="30" t="s">
         <v>108</v>
       </c>
-      <c r="F5" s="32">
+      <c r="F5" s="31">
         <v>22</v>
       </c>
-      <c r="G5" s="32">
+      <c r="G5" s="31">
         <v>22</v>
       </c>
-      <c r="H5" s="32">
+      <c r="H5" s="31">
         <v>22</v>
       </c>
-      <c r="I5" s="32">
+      <c r="I5" s="31">
         <v>22</v>
       </c>
-      <c r="J5" s="32">
+      <c r="J5" s="31">
         <v>13</v>
       </c>
-      <c r="K5" s="32">
+      <c r="K5" s="31">
         <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="33.75" customHeight="1">
-      <c r="A6" s="66"/>
-      <c r="B6" s="80" t="s">
+      <c r="A6" s="62"/>
+      <c r="B6" s="76" t="s">
         <v>112</v>
       </c>
-      <c r="C6" s="81"/>
-      <c r="D6" s="82"/>
-      <c r="E6" s="31" t="s">
+      <c r="C6" s="77"/>
+      <c r="D6" s="78"/>
+      <c r="E6" s="30" t="s">
         <v>109</v>
       </c>
-      <c r="F6" s="32" t="s">
+      <c r="F6" s="31" t="s">
         <v>106</v>
       </c>
-      <c r="G6" s="32" t="s">
+      <c r="G6" s="31" t="s">
         <v>125</v>
       </c>
-      <c r="H6" s="32" t="s">
+      <c r="H6" s="31" t="s">
         <v>126</v>
       </c>
-      <c r="I6" s="32" t="s">
+      <c r="I6" s="31" t="s">
         <v>136</v>
       </c>
-      <c r="J6" s="32" t="s">
+      <c r="J6" s="31" t="s">
         <v>125</v>
       </c>
-      <c r="K6" s="32" t="s">
+      <c r="K6" s="31" t="s">
         <v>126</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="31.5">
-      <c r="A7" s="66"/>
-      <c r="B7" s="71" t="s">
+      <c r="A7" s="62"/>
+      <c r="B7" s="67" t="s">
         <v>110</v>
       </c>
-      <c r="C7" s="72"/>
-      <c r="D7" s="35" t="s">
+      <c r="C7" s="68"/>
+      <c r="D7" s="34" t="s">
         <v>114</v>
       </c>
-      <c r="E7" s="31" t="s">
+      <c r="E7" s="30" t="s">
         <v>115</v>
       </c>
-      <c r="F7" s="32" t="s">
+      <c r="F7" s="31" t="s">
         <v>116</v>
       </c>
-      <c r="G7" s="32" t="s">
+      <c r="G7" s="31" t="s">
         <v>128</v>
       </c>
-      <c r="H7" s="32" t="s">
+      <c r="H7" s="31" t="s">
         <v>127</v>
       </c>
-      <c r="I7" s="32" t="s">
+      <c r="I7" s="31" t="s">
         <v>137</v>
       </c>
-      <c r="J7" s="32" t="s">
+      <c r="J7" s="31" t="s">
         <v>128</v>
       </c>
-      <c r="K7" s="32" t="s">
+      <c r="K7" s="31" t="s">
         <v>127</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="30">
-      <c r="A8" s="66"/>
-      <c r="B8" s="73"/>
-      <c r="C8" s="74"/>
-      <c r="D8" s="36" t="s">
+      <c r="A8" s="62"/>
+      <c r="B8" s="69"/>
+      <c r="C8" s="70"/>
+      <c r="D8" s="35" t="s">
         <v>120</v>
       </c>
-      <c r="E8" s="31" t="s">
+      <c r="E8" s="30" t="s">
         <v>117</v>
       </c>
-      <c r="F8" s="32" t="s">
+      <c r="F8" s="31" t="s">
         <v>124</v>
       </c>
-      <c r="G8" s="32" t="s">
+      <c r="G8" s="31" t="s">
         <v>130</v>
       </c>
-      <c r="H8" s="32" t="s">
+      <c r="H8" s="31" t="s">
         <v>129</v>
       </c>
-      <c r="I8" s="32" t="s">
+      <c r="I8" s="31" t="s">
         <v>138</v>
       </c>
-      <c r="J8" s="32" t="s">
+      <c r="J8" s="31" t="s">
         <v>139</v>
       </c>
-      <c r="K8" s="32" t="s">
+      <c r="K8" s="31" t="s">
         <v>140</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="31.5">
-      <c r="A9" s="66"/>
-      <c r="B9" s="73"/>
-      <c r="C9" s="74"/>
-      <c r="D9" s="35" t="s">
+      <c r="A9" s="62"/>
+      <c r="B9" s="69"/>
+      <c r="C9" s="70"/>
+      <c r="D9" s="34" t="s">
         <v>121</v>
       </c>
-      <c r="E9" s="31" t="s">
+      <c r="E9" s="30" t="s">
         <v>118</v>
       </c>
-      <c r="F9" s="32">
+      <c r="F9" s="31">
         <v>345</v>
       </c>
-      <c r="G9" s="32">
+      <c r="G9" s="31">
         <v>567</v>
       </c>
-      <c r="H9" s="32">
+      <c r="H9" s="31">
         <v>2100</v>
       </c>
-      <c r="I9" s="32">
+      <c r="I9" s="31">
         <v>452</v>
       </c>
-      <c r="J9" s="32">
+      <c r="J9" s="31">
         <v>643</v>
       </c>
-      <c r="K9" s="32">
+      <c r="K9" s="31">
         <v>783</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="31.5">
-      <c r="A10" s="67"/>
-      <c r="B10" s="75"/>
-      <c r="C10" s="76"/>
-      <c r="D10" s="35" t="s">
+      <c r="A10" s="63"/>
+      <c r="B10" s="71"/>
+      <c r="C10" s="72"/>
+      <c r="D10" s="34" t="s">
         <v>122</v>
       </c>
-      <c r="E10" s="31" t="s">
+      <c r="E10" s="30" t="s">
         <v>119</v>
       </c>
-      <c r="F10" s="33" t="s">
+      <c r="F10" s="32" t="s">
         <v>123</v>
       </c>
-      <c r="G10" s="34">
+      <c r="G10" s="33">
         <v>0.45</v>
       </c>
-      <c r="H10" s="34">
+      <c r="H10" s="33">
         <v>0.65</v>
       </c>
-      <c r="I10" s="34">
+      <c r="I10" s="33">
         <v>0.67</v>
       </c>
-      <c r="J10" s="34">
+      <c r="J10" s="33">
         <v>0.45</v>
       </c>
-      <c r="K10" s="34">
+      <c r="K10" s="33">
         <v>0.34</v>
       </c>
     </row>
@@ -3964,11 +3983,11 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:8">
-      <c r="F3" s="91" t="s">
+      <c r="F3" s="87" t="s">
         <v>40</v>
       </c>
-      <c r="G3" s="92"/>
-      <c r="H3" s="92"/>
+      <c r="G3" s="88"/>
+      <c r="H3" s="88"/>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" s="6" t="s">
@@ -3986,215 +4005,215 @@
       <c r="E4" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="F4" s="37" t="s">
+      <c r="F4" s="36" t="s">
         <v>142</v>
       </c>
-      <c r="G4" s="37" t="s">
+      <c r="G4" s="36" t="s">
         <v>143</v>
       </c>
-      <c r="H4" s="37" t="s">
+      <c r="H4" s="36" t="s">
         <v>144</v>
       </c>
     </row>
     <row r="5" spans="1:8">
-      <c r="A5" s="89" t="s">
+      <c r="A5" s="85" t="s">
         <v>28</v>
       </c>
-      <c r="B5" s="24" t="s">
+      <c r="B5" s="23" t="s">
         <v>150</v>
       </c>
-      <c r="C5" s="26" t="s">
+      <c r="C5" s="25" t="s">
         <v>149</v>
       </c>
-      <c r="D5" s="23">
+      <c r="D5" s="22">
         <v>1</v>
       </c>
       <c r="E5" s="6" t="s">
         <v>148</v>
       </c>
-      <c r="F5" s="41" t="s">
+      <c r="F5" s="40" t="s">
         <v>163</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>164</v>
       </c>
-      <c r="H5" s="42" t="s">
+      <c r="H5" s="41" t="s">
         <v>145</v>
       </c>
     </row>
     <row r="6" spans="1:8">
-      <c r="A6" s="89"/>
-      <c r="B6" s="24" t="s">
+      <c r="A6" s="85"/>
+      <c r="B6" s="23" t="s">
         <v>151</v>
       </c>
-      <c r="C6" s="26" t="s">
+      <c r="C6" s="25" t="s">
         <v>149</v>
       </c>
-      <c r="D6" s="23">
+      <c r="D6" s="22">
         <v>2</v>
       </c>
       <c r="E6" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="F6" s="41" t="s">
+      <c r="F6" s="40" t="s">
         <v>141</v>
       </c>
       <c r="G6" s="2" t="s">
         <v>164</v>
       </c>
-      <c r="H6" s="42" t="s">
+      <c r="H6" s="41" t="s">
         <v>145</v>
       </c>
     </row>
     <row r="7" spans="1:8">
-      <c r="A7" s="89"/>
-      <c r="B7" s="24" t="s">
+      <c r="A7" s="85"/>
+      <c r="B7" s="23" t="s">
         <v>25</v>
       </c>
-      <c r="C7" s="26" t="s">
+      <c r="C7" s="25" t="s">
         <v>149</v>
       </c>
-      <c r="D7" s="23">
+      <c r="D7" s="22">
         <v>3</v>
       </c>
       <c r="E7" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="F7" s="41">
+      <c r="F7" s="40">
         <v>2</v>
       </c>
       <c r="G7" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="H7" s="42" t="s">
+      <c r="H7" s="41" t="s">
         <v>145</v>
       </c>
     </row>
     <row r="8" spans="1:8">
-      <c r="A8" s="89"/>
-      <c r="B8" s="24" t="s">
+      <c r="A8" s="85"/>
+      <c r="B8" s="23" t="s">
         <v>27</v>
       </c>
-      <c r="C8" s="26" t="s">
+      <c r="C8" s="25" t="s">
         <v>149</v>
       </c>
-      <c r="D8" s="23">
+      <c r="D8" s="22">
         <v>4</v>
       </c>
       <c r="E8" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="F8" s="41" t="s">
+      <c r="F8" s="40" t="s">
         <v>38</v>
       </c>
       <c r="G8" s="2" t="s">
         <v>164</v>
       </c>
-      <c r="H8" s="42" t="s">
+      <c r="H8" s="41" t="s">
         <v>145</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="30">
-      <c r="A9" s="90" t="s">
+      <c r="A9" s="86" t="s">
         <v>152</v>
       </c>
-      <c r="B9" s="24" t="s">
+      <c r="B9" s="23" t="s">
         <v>31</v>
       </c>
-      <c r="C9" s="26" t="s">
+      <c r="C9" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="D9" s="23">
+      <c r="D9" s="22">
         <v>5</v>
       </c>
       <c r="E9" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="F9" s="41" t="s">
+      <c r="F9" s="40" t="s">
         <v>3</v>
       </c>
       <c r="G9" s="2"/>
-      <c r="H9" s="42"/>
+      <c r="H9" s="41"/>
     </row>
     <row r="10" spans="1:8">
-      <c r="A10" s="90"/>
-      <c r="B10" s="24" t="s">
+      <c r="A10" s="86"/>
+      <c r="B10" s="23" t="s">
         <v>153</v>
       </c>
-      <c r="C10" s="26" t="s">
+      <c r="C10" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="D10" s="23">
+      <c r="D10" s="22">
         <v>6</v>
       </c>
       <c r="E10" s="6" t="s">
         <v>157</v>
       </c>
-      <c r="F10" s="41" t="s">
+      <c r="F10" s="40" t="s">
         <v>17</v>
       </c>
       <c r="G10" s="2"/>
-      <c r="H10" s="42"/>
+      <c r="H10" s="41"/>
     </row>
     <row r="11" spans="1:8">
-      <c r="A11" s="90"/>
-      <c r="B11" s="24" t="s">
+      <c r="A11" s="86"/>
+      <c r="B11" s="23" t="s">
         <v>154</v>
       </c>
-      <c r="C11" s="26" t="s">
+      <c r="C11" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="D11" s="23">
+      <c r="D11" s="22">
         <v>7</v>
       </c>
       <c r="E11" s="6" t="s">
         <v>158</v>
       </c>
-      <c r="F11" s="41">
+      <c r="F11" s="40">
         <v>4.4000000000000004</v>
       </c>
       <c r="G11" s="2"/>
-      <c r="H11" s="42"/>
+      <c r="H11" s="41"/>
     </row>
     <row r="12" spans="1:8">
-      <c r="A12" s="90"/>
-      <c r="B12" s="24" t="s">
+      <c r="A12" s="86"/>
+      <c r="B12" s="23" t="s">
         <v>155</v>
       </c>
-      <c r="C12" s="26" t="s">
+      <c r="C12" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="D12" s="23">
+      <c r="D12" s="22">
         <v>8</v>
       </c>
       <c r="E12" s="6" t="s">
         <v>159</v>
       </c>
-      <c r="F12" s="41" t="s">
+      <c r="F12" s="40" t="s">
         <v>18</v>
       </c>
       <c r="G12" s="2"/>
-      <c r="H12" s="42"/>
+      <c r="H12" s="41"/>
     </row>
     <row r="13" spans="1:8">
-      <c r="A13" s="90"/>
-      <c r="B13" s="25" t="s">
+      <c r="A13" s="86"/>
+      <c r="B13" s="24" t="s">
         <v>156</v>
       </c>
-      <c r="C13" s="26" t="s">
+      <c r="C13" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="D13" s="23">
+      <c r="D13" s="22">
         <v>9</v>
       </c>
       <c r="E13" s="6" t="s">
         <v>161</v>
       </c>
-      <c r="F13" s="41" t="s">
+      <c r="F13" s="40" t="s">
         <v>160</v>
       </c>
       <c r="G13" s="2"/>
-      <c r="H13" s="42"/>
+      <c r="H13" s="41"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -4227,34 +4246,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17">
-      <c r="B1" s="38" t="s">
+      <c r="B1" s="37" t="s">
         <v>146</v>
       </c>
-      <c r="C1" s="93" t="s">
+      <c r="C1" s="89" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="94"/>
-      <c r="E1" s="95"/>
-      <c r="F1" s="93" t="s">
+      <c r="D1" s="90"/>
+      <c r="E1" s="91"/>
+      <c r="F1" s="89" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="94"/>
-      <c r="H1" s="95"/>
-      <c r="I1" s="93" t="s">
+      <c r="G1" s="90"/>
+      <c r="H1" s="91"/>
+      <c r="I1" s="89" t="s">
         <v>65</v>
       </c>
-      <c r="J1" s="94"/>
-      <c r="K1" s="95"/>
-      <c r="L1" s="96" t="s">
+      <c r="J1" s="90"/>
+      <c r="K1" s="91"/>
+      <c r="L1" s="92" t="s">
         <v>66</v>
       </c>
-      <c r="M1" s="97"/>
-      <c r="N1" s="97"/>
-      <c r="O1" s="93" t="s">
+      <c r="M1" s="93"/>
+      <c r="N1" s="93"/>
+      <c r="O1" s="89" t="s">
         <v>131</v>
       </c>
-      <c r="P1" s="94"/>
-      <c r="Q1" s="95"/>
+      <c r="P1" s="90"/>
+      <c r="Q1" s="91"/>
     </row>
     <row r="2" spans="1:17">
       <c r="A2" s="4" t="s">
@@ -4263,54 +4282,54 @@
       <c r="B2" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="C2" s="37" t="s">
+      <c r="C2" s="36" t="s">
         <v>142</v>
       </c>
-      <c r="D2" s="37" t="s">
+      <c r="D2" s="36" t="s">
         <v>143</v>
       </c>
-      <c r="E2" s="37" t="s">
+      <c r="E2" s="36" t="s">
         <v>144</v>
       </c>
-      <c r="F2" s="37" t="s">
+      <c r="F2" s="36" t="s">
         <v>142</v>
       </c>
-      <c r="G2" s="37" t="s">
+      <c r="G2" s="36" t="s">
         <v>143</v>
       </c>
-      <c r="H2" s="37" t="s">
+      <c r="H2" s="36" t="s">
         <v>144</v>
       </c>
-      <c r="I2" s="37" t="s">
+      <c r="I2" s="36" t="s">
         <v>142</v>
       </c>
-      <c r="J2" s="37" t="s">
+      <c r="J2" s="36" t="s">
         <v>143</v>
       </c>
-      <c r="K2" s="37" t="s">
+      <c r="K2" s="36" t="s">
         <v>144</v>
       </c>
-      <c r="L2" s="37" t="s">
+      <c r="L2" s="36" t="s">
         <v>142</v>
       </c>
-      <c r="M2" s="37" t="s">
+      <c r="M2" s="36" t="s">
         <v>143</v>
       </c>
-      <c r="N2" s="37" t="s">
+      <c r="N2" s="36" t="s">
         <v>144</v>
       </c>
-      <c r="O2" s="37" t="s">
+      <c r="O2" s="36" t="s">
         <v>142</v>
       </c>
-      <c r="P2" s="37" t="s">
+      <c r="P2" s="36" t="s">
         <v>143</v>
       </c>
-      <c r="Q2" s="37" t="s">
+      <c r="Q2" s="36" t="s">
         <v>144</v>
       </c>
     </row>
     <row r="3" spans="1:17">
-      <c r="A3" s="23" t="s">
+      <c r="A3" s="22" t="s">
         <v>75</v>
       </c>
       <c r="B3" s="4" t="s">
@@ -4368,7 +4387,7 @@
       </c>
     </row>
     <row r="4" spans="1:17">
-      <c r="A4" s="23" t="s">
+      <c r="A4" s="22" t="s">
         <v>76</v>
       </c>
       <c r="B4" s="4" t="s">
@@ -4426,7 +4445,7 @@
       </c>
     </row>
     <row r="5" spans="1:17">
-      <c r="A5" s="39" t="s">
+      <c r="A5" s="38" t="s">
         <v>77</v>
       </c>
       <c r="B5" s="4" t="s">
@@ -4459,13 +4478,13 @@
       </c>
     </row>
     <row r="6" spans="1:17">
-      <c r="A6" s="40" t="s">
+      <c r="A6" s="39" t="s">
         <v>78</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C6" s="30" t="s">
+      <c r="C6" s="29" t="s">
         <v>100</v>
       </c>
       <c r="D6" s="8" t="str">
@@ -4485,7 +4504,7 @@
       <c r="H6" s="8" t="s">
         <v>145</v>
       </c>
-      <c r="I6" s="29" t="b">
+      <c r="I6" s="28" t="b">
         <v>1</v>
       </c>
       <c r="J6" s="8" t="b">
@@ -4572,29 +4591,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14">
-      <c r="B1" s="38" t="s">
+      <c r="B1" s="37" t="s">
         <v>146</v>
       </c>
-      <c r="C1" s="93" t="s">
+      <c r="C1" s="89" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="94"/>
-      <c r="E1" s="95"/>
-      <c r="F1" s="93" t="s">
+      <c r="D1" s="90"/>
+      <c r="E1" s="91"/>
+      <c r="F1" s="89" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="94"/>
-      <c r="H1" s="95"/>
-      <c r="I1" s="93" t="s">
+      <c r="G1" s="90"/>
+      <c r="H1" s="91"/>
+      <c r="I1" s="89" t="s">
         <v>65</v>
       </c>
-      <c r="J1" s="94"/>
-      <c r="K1" s="95"/>
-      <c r="L1" s="96" t="s">
+      <c r="J1" s="90"/>
+      <c r="K1" s="91"/>
+      <c r="L1" s="92" t="s">
         <v>66</v>
       </c>
-      <c r="M1" s="97"/>
-      <c r="N1" s="97"/>
+      <c r="M1" s="93"/>
+      <c r="N1" s="93"/>
     </row>
     <row r="2" spans="1:14">
       <c r="A2" s="4" t="s">
@@ -4603,61 +4622,61 @@
       <c r="B2" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="C2" s="37" t="s">
+      <c r="C2" s="36" t="s">
         <v>142</v>
       </c>
-      <c r="D2" s="37" t="s">
+      <c r="D2" s="36" t="s">
         <v>143</v>
       </c>
-      <c r="E2" s="37" t="s">
+      <c r="E2" s="36" t="s">
         <v>144</v>
       </c>
-      <c r="F2" s="37" t="s">
+      <c r="F2" s="36" t="s">
         <v>142</v>
       </c>
-      <c r="G2" s="37" t="s">
+      <c r="G2" s="36" t="s">
         <v>143</v>
       </c>
-      <c r="H2" s="37" t="s">
+      <c r="H2" s="36" t="s">
         <v>144</v>
       </c>
-      <c r="I2" s="37" t="s">
+      <c r="I2" s="36" t="s">
         <v>142</v>
       </c>
-      <c r="J2" s="37" t="s">
+      <c r="J2" s="36" t="s">
         <v>143</v>
       </c>
-      <c r="K2" s="37" t="s">
+      <c r="K2" s="36" t="s">
         <v>144</v>
       </c>
-      <c r="L2" s="37" t="s">
+      <c r="L2" s="36" t="s">
         <v>142</v>
       </c>
-      <c r="M2" s="37" t="s">
+      <c r="M2" s="36" t="s">
         <v>143</v>
       </c>
-      <c r="N2" s="37" t="s">
+      <c r="N2" s="36" t="s">
         <v>144</v>
       </c>
     </row>
     <row r="3" spans="1:14">
       <c r="A3" s="4"/>
       <c r="B3" s="5"/>
-      <c r="C3" s="37"/>
-      <c r="D3" s="37"/>
-      <c r="E3" s="37"/>
-      <c r="F3" s="37"/>
-      <c r="G3" s="37"/>
-      <c r="H3" s="37"/>
-      <c r="I3" s="37"/>
-      <c r="J3" s="37"/>
-      <c r="K3" s="37"/>
-      <c r="L3" s="37"/>
-      <c r="M3" s="37"/>
-      <c r="N3" s="37"/>
+      <c r="C3" s="36"/>
+      <c r="D3" s="36"/>
+      <c r="E3" s="36"/>
+      <c r="F3" s="36"/>
+      <c r="G3" s="36"/>
+      <c r="H3" s="36"/>
+      <c r="I3" s="36"/>
+      <c r="J3" s="36"/>
+      <c r="K3" s="36"/>
+      <c r="L3" s="36"/>
+      <c r="M3" s="36"/>
+      <c r="N3" s="36"/>
     </row>
     <row r="4" spans="1:14">
-      <c r="A4" s="23" t="s">
+      <c r="A4" s="22" t="s">
         <v>75</v>
       </c>
       <c r="B4" s="4" t="s">
@@ -4705,7 +4724,7 @@
       </c>
     </row>
     <row r="5" spans="1:14">
-      <c r="A5" s="23"/>
+      <c r="A5" s="22"/>
       <c r="B5" s="4" t="s">
         <v>83</v>
       </c>
@@ -4715,12 +4734,12 @@
       <c r="F5" s="8"/>
       <c r="G5" s="8"/>
       <c r="H5" s="8"/>
-      <c r="I5" s="43"/>
-      <c r="J5" s="43"/>
-      <c r="K5" s="43"/>
-      <c r="L5" s="43"/>
-      <c r="M5" s="43"/>
-      <c r="N5" s="43"/>
+      <c r="I5" s="42"/>
+      <c r="J5" s="42"/>
+      <c r="K5" s="42"/>
+      <c r="L5" s="42"/>
+      <c r="M5" s="42"/>
+      <c r="N5" s="42"/>
     </row>
     <row r="6" spans="1:14">
       <c r="A6" s="9" t="s">
@@ -4730,7 +4749,7 @@
       <c r="C6" s="4"/>
       <c r="D6" s="8"/>
       <c r="E6" s="8"/>
-      <c r="F6" s="19"/>
+      <c r="F6" s="18"/>
       <c r="G6" s="8"/>
       <c r="H6" s="8"/>
     </row>
@@ -4740,12 +4759,12 @@
       <c r="C7" s="4"/>
       <c r="D7" s="8"/>
       <c r="E7" s="8"/>
-      <c r="F7" s="19"/>
+      <c r="F7" s="18"/>
       <c r="G7" s="8"/>
       <c r="H7" s="8"/>
     </row>
     <row r="8" spans="1:14">
-      <c r="A8" s="23" t="s">
+      <c r="A8" s="22" t="s">
         <v>76</v>
       </c>
       <c r="B8" s="4" t="s">
@@ -4793,7 +4812,7 @@
       </c>
     </row>
     <row r="9" spans="1:14">
-      <c r="A9" s="39" t="s">
+      <c r="A9" s="38" t="s">
         <v>77</v>
       </c>
       <c r="B9" s="4" t="s">
@@ -4821,13 +4840,13 @@
       </c>
     </row>
     <row r="10" spans="1:14">
-      <c r="A10" s="40" t="s">
+      <c r="A10" s="39" t="s">
         <v>78</v>
       </c>
       <c r="B10" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C10" s="30" t="s">
+      <c r="C10" s="29" t="s">
         <v>100</v>
       </c>
       <c r="D10" s="8" t="str">
@@ -4847,7 +4866,7 @@
       <c r="H10" s="8" t="s">
         <v>145</v>
       </c>
-      <c r="I10" s="29" t="b">
+      <c r="I10" s="28" t="b">
         <v>1</v>
       </c>
       <c r="J10" s="8" t="b">

</xml_diff>

<commit_message>
fix headermap error, pass test
</commit_message>
<xml_diff>
--- a/JavaExcelBDD/src/test/resources/ExcelBDD.xlsx
+++ b/JavaExcelBDD/src/test/resources/ExcelBDD.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/2fe8b90741a02718/Git/SimpleOpenExcelBDD/JavaExcelBDD/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="55" documentId="13_ncr:1_{2BC08F18-7250-451B-B716-B852607D4077}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{99C28B43-8604-40E7-9B9A-C5C8F69C8097}"/>
+  <xr:revisionPtr revIDLastSave="60" documentId="13_ncr:1_{2BC08F18-7250-451B-B716-B852607D4077}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EBD998DE-837C-4232-A43C-1082D17D6B12}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{965C72BA-AC7B-4020-96A1-B4855C2F0853}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="9" xr2:uid="{965C72BA-AC7B-4020-96A1-B4855C2F0853}"/>
   </bookViews>
   <sheets>
     <sheet name="SimpleOpenBDD" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="623" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="624" uniqueCount="169">
   <si>
     <t>Role</t>
   </si>
@@ -543,12 +543,6 @@
   </si>
   <si>
     <t>GUI Prototype</t>
-  </si>
-  <si>
-    <t>V1.6</t>
-  </si>
-  <si>
-    <t>V2.6</t>
   </si>
   <si>
     <t>Scenario1b</t>
@@ -953,6 +947,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
@@ -1108,9 +1105,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1626,7 +1620,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E1F2AA4-76D9-4C80-95B2-1FE7E77EF6CA}">
   <dimension ref="A1:H18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
@@ -1913,16 +1907,16 @@
       <c r="H11" s="7"/>
     </row>
     <row r="12" spans="1:8" ht="45">
-      <c r="A12" s="43">
+      <c r="A12" s="44">
         <v>11</v>
       </c>
       <c r="B12" s="23" t="s">
         <v>89</v>
       </c>
-      <c r="C12" s="46" t="s">
+      <c r="C12" s="47" t="s">
         <v>5</v>
       </c>
-      <c r="D12" s="47" t="s">
+      <c r="D12" s="48" t="s">
         <v>86</v>
       </c>
       <c r="E12" s="7">
@@ -1939,36 +1933,36 @@
       </c>
     </row>
     <row r="13" spans="1:8">
-      <c r="A13" s="44"/>
+      <c r="A13" s="45"/>
       <c r="B13" s="20" t="s">
         <v>97</v>
       </c>
-      <c r="C13" s="46"/>
-      <c r="D13" s="48"/>
+      <c r="C13" s="47"/>
+      <c r="D13" s="49"/>
       <c r="E13" s="7"/>
       <c r="F13" s="7"/>
       <c r="G13" s="7"/>
       <c r="H13" s="7"/>
     </row>
     <row r="14" spans="1:8">
-      <c r="A14" s="44"/>
+      <c r="A14" s="45"/>
       <c r="B14" s="20" t="s">
         <v>84</v>
       </c>
-      <c r="C14" s="46"/>
-      <c r="D14" s="48"/>
+      <c r="C14" s="47"/>
+      <c r="D14" s="49"/>
       <c r="E14" s="7"/>
       <c r="F14" s="7"/>
       <c r="G14" s="7"/>
       <c r="H14" s="7"/>
     </row>
     <row r="15" spans="1:8">
-      <c r="A15" s="45"/>
+      <c r="A15" s="46"/>
       <c r="B15" s="21" t="s">
         <v>85</v>
       </c>
-      <c r="C15" s="46"/>
-      <c r="D15" s="49"/>
+      <c r="C15" s="47"/>
+      <c r="D15" s="50"/>
       <c r="E15" s="7"/>
       <c r="F15" s="7"/>
       <c r="G15" s="7"/>
@@ -2030,14 +2024,14 @@
       <c r="A18" s="2">
         <v>14</v>
       </c>
-      <c r="B18" s="95" t="s">
-        <v>169</v>
+      <c r="B18" s="43" t="s">
+        <v>167</v>
       </c>
       <c r="C18" s="25" t="s">
         <v>5</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="E18" s="7">
         <v>4</v>
@@ -2067,8 +2061,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27202F44-224C-40C0-ACC3-02135A9560D7}">
   <dimension ref="A1:V11"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="T2" sqref="T2"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="T4" sqref="T4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2089,36 +2083,36 @@
       <c r="D1" s="37" t="s">
         <v>146</v>
       </c>
-      <c r="E1" s="89" t="s">
+      <c r="E1" s="90" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="90"/>
-      <c r="G1" s="91"/>
-      <c r="H1" s="89" t="s">
+      <c r="F1" s="91"/>
+      <c r="G1" s="92"/>
+      <c r="H1" s="90" t="s">
         <v>4</v>
       </c>
-      <c r="I1" s="90"/>
-      <c r="J1" s="91"/>
-      <c r="K1" s="89" t="s">
+      <c r="I1" s="91"/>
+      <c r="J1" s="92"/>
+      <c r="K1" s="90" t="s">
         <v>65</v>
       </c>
-      <c r="L1" s="90"/>
-      <c r="M1" s="91"/>
-      <c r="N1" s="94" t="s">
+      <c r="L1" s="91"/>
+      <c r="M1" s="92"/>
+      <c r="N1" s="95" t="s">
         <v>66</v>
       </c>
-      <c r="O1" s="94"/>
-      <c r="P1" s="94"/>
-      <c r="Q1" s="89" t="s">
+      <c r="O1" s="95"/>
+      <c r="P1" s="95"/>
+      <c r="Q1" s="90" t="s">
         <v>131</v>
       </c>
-      <c r="R1" s="90"/>
-      <c r="S1" s="91"/>
-      <c r="T1" s="89" t="s">
-        <v>168</v>
-      </c>
-      <c r="U1" s="90"/>
-      <c r="V1" s="91"/>
+      <c r="R1" s="91"/>
+      <c r="S1" s="92"/>
+      <c r="T1" s="90" t="s">
+        <v>166</v>
+      </c>
+      <c r="U1" s="91"/>
+      <c r="V1" s="92"/>
     </row>
     <row r="2" spans="1:22">
       <c r="A2" s="4" t="s">
@@ -2250,11 +2244,11 @@
         <v>145</v>
       </c>
       <c r="T3" s="8" t="s">
-        <v>166</v>
+        <v>17</v>
       </c>
       <c r="U3" s="8" t="str">
         <f>T3</f>
-        <v>V1.6</v>
+        <v>V1.1</v>
       </c>
       <c r="V3" s="8" t="s">
         <v>145</v>
@@ -2322,11 +2316,11 @@
         <v>145</v>
       </c>
       <c r="T4" s="8" t="s">
-        <v>167</v>
+        <v>21</v>
       </c>
       <c r="U4" s="8" t="str">
-        <f t="shared" ref="U4" si="5">T4</f>
-        <v>V2.6</v>
+        <f t="shared" ref="U4:U6" si="5">T4</f>
+        <v>V2.1</v>
       </c>
       <c r="V4" s="8" t="s">
         <v>145</v>
@@ -2435,12 +2429,12 @@
       <c r="S6" s="8" t="s">
         <v>145</v>
       </c>
-      <c r="T6" s="7">
-        <v>4.5999999999999996</v>
-      </c>
-      <c r="U6" s="8">
+      <c r="T6" s="29" t="s">
+        <v>100</v>
+      </c>
+      <c r="U6" s="8" t="str">
         <f t="shared" ref="U6" si="7">T6</f>
-        <v>4.5999999999999996</v>
+        <v>2021/4/30</v>
       </c>
       <c r="V6" s="8" t="s">
         <v>145</v>
@@ -2508,31 +2502,31 @@
       <c r="D3" s="37" t="s">
         <v>146</v>
       </c>
-      <c r="E3" s="89" t="s">
+      <c r="E3" s="90" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="90"/>
-      <c r="G3" s="91"/>
-      <c r="H3" s="89" t="s">
+      <c r="F3" s="91"/>
+      <c r="G3" s="92"/>
+      <c r="H3" s="90" t="s">
         <v>4</v>
       </c>
-      <c r="I3" s="90"/>
-      <c r="J3" s="91"/>
-      <c r="K3" s="89" t="s">
+      <c r="I3" s="91"/>
+      <c r="J3" s="92"/>
+      <c r="K3" s="90" t="s">
         <v>65</v>
       </c>
-      <c r="L3" s="90"/>
-      <c r="M3" s="91"/>
-      <c r="N3" s="94" t="s">
+      <c r="L3" s="91"/>
+      <c r="M3" s="92"/>
+      <c r="N3" s="95" t="s">
         <v>66</v>
       </c>
-      <c r="O3" s="94"/>
-      <c r="P3" s="94"/>
-      <c r="Q3" s="89" t="s">
+      <c r="O3" s="95"/>
+      <c r="P3" s="95"/>
+      <c r="Q3" s="90" t="s">
         <v>131</v>
       </c>
-      <c r="R3" s="90"/>
-      <c r="S3" s="91"/>
+      <c r="R3" s="91"/>
+      <c r="S3" s="92"/>
     </row>
     <row r="4" spans="1:19">
       <c r="A4" s="4" t="s">
@@ -2965,7 +2959,7 @@
       <c r="G6" s="18"/>
     </row>
     <row r="7" spans="1:7">
-      <c r="A7" s="50" t="s">
+      <c r="A7" s="51" t="s">
         <v>77</v>
       </c>
       <c r="B7" s="4" t="s">
@@ -2978,7 +2972,7 @@
       <c r="G7" s="18"/>
     </row>
     <row r="8" spans="1:7">
-      <c r="A8" s="51"/>
+      <c r="A8" s="52"/>
       <c r="B8" s="4" t="s">
         <v>83</v>
       </c>
@@ -2989,7 +2983,7 @@
       <c r="G8" s="18"/>
     </row>
     <row r="9" spans="1:7">
-      <c r="A9" s="52" t="s">
+      <c r="A9" s="53" t="s">
         <v>78</v>
       </c>
       <c r="B9" s="4" t="s">
@@ -3012,7 +3006,7 @@
       </c>
     </row>
     <row r="10" spans="1:7">
-      <c r="A10" s="53"/>
+      <c r="A10" s="54"/>
       <c r="B10" s="15" t="s">
         <v>83</v>
       </c>
@@ -3284,15 +3278,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="54" t="s">
+      <c r="A1" s="55" t="s">
         <v>43</v>
       </c>
-      <c r="B1" s="54"/>
-      <c r="C1" s="54"/>
-      <c r="D1" s="54"/>
-      <c r="E1" s="54"/>
-      <c r="F1" s="54"/>
-      <c r="G1" s="54"/>
+      <c r="B1" s="55"/>
+      <c r="C1" s="55"/>
+      <c r="D1" s="55"/>
+      <c r="E1" s="55"/>
+      <c r="F1" s="55"/>
+      <c r="G1" s="55"/>
       <c r="H1" s="2"/>
     </row>
     <row r="2" spans="1:8">
@@ -3328,7 +3322,7 @@
       <c r="B3" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="C3" s="55" t="s">
+      <c r="C3" s="56" t="s">
         <v>46</v>
       </c>
       <c r="D3" s="4" t="s">
@@ -3354,7 +3348,7 @@
       <c r="B4" s="9" t="s">
         <v>76</v>
       </c>
-      <c r="C4" s="56"/>
+      <c r="C4" s="57"/>
       <c r="D4" s="4" t="s">
         <v>14</v>
       </c>
@@ -3378,7 +3372,7 @@
       <c r="B5" s="9" t="s">
         <v>77</v>
       </c>
-      <c r="C5" s="57"/>
+      <c r="C5" s="58"/>
       <c r="D5" s="4" t="s">
         <v>15</v>
       </c>
@@ -3456,42 +3450,42 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
-      <c r="A1" s="60" t="s">
+      <c r="A1" s="61" t="s">
         <v>50</v>
       </c>
-      <c r="B1" s="60"/>
-      <c r="C1" s="54" t="s">
+      <c r="B1" s="61"/>
+      <c r="C1" s="55" t="s">
         <v>64</v>
       </c>
-      <c r="D1" s="54"/>
+      <c r="D1" s="55"/>
       <c r="E1" s="14" t="s">
         <v>51</v>
       </c>
-      <c r="F1" s="58" t="s">
+      <c r="F1" s="59" t="s">
         <v>52</v>
       </c>
-      <c r="G1" s="59"/>
-      <c r="H1" s="59"/>
-      <c r="I1" s="59"/>
+      <c r="G1" s="60"/>
+      <c r="H1" s="60"/>
+      <c r="I1" s="60"/>
     </row>
     <row r="2" spans="1:9">
-      <c r="A2" s="60" t="s">
+      <c r="A2" s="61" t="s">
         <v>53</v>
       </c>
-      <c r="B2" s="60"/>
-      <c r="C2" s="66" t="s">
+      <c r="B2" s="61"/>
+      <c r="C2" s="67" t="s">
         <v>49</v>
       </c>
-      <c r="D2" s="66"/>
+      <c r="D2" s="67"/>
       <c r="E2" s="11" t="s">
         <v>80</v>
       </c>
-      <c r="F2" s="64" t="s">
+      <c r="F2" s="65" t="s">
         <v>81</v>
       </c>
-      <c r="G2" s="64"/>
-      <c r="H2" s="64"/>
-      <c r="I2" s="65"/>
+      <c r="G2" s="65"/>
+      <c r="H2" s="65"/>
+      <c r="I2" s="66"/>
     </row>
     <row r="3" spans="1:9">
       <c r="A3" s="13" t="s">
@@ -3523,16 +3517,16 @@
       </c>
     </row>
     <row r="4" spans="1:9" ht="69.95" customHeight="1">
-      <c r="A4" s="61" t="s">
+      <c r="A4" s="62" t="s">
         <v>57</v>
       </c>
       <c r="B4" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="C4" s="61" t="s">
+      <c r="C4" s="62" t="s">
         <v>48</v>
       </c>
-      <c r="D4" s="55" t="s">
+      <c r="D4" s="56" t="s">
         <v>46</v>
       </c>
       <c r="E4" s="4" t="s">
@@ -3552,12 +3546,12 @@
       </c>
     </row>
     <row r="5" spans="1:9" ht="69.95" customHeight="1">
-      <c r="A5" s="62"/>
+      <c r="A5" s="63"/>
       <c r="B5" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="C5" s="62"/>
-      <c r="D5" s="56"/>
+      <c r="C5" s="63"/>
+      <c r="D5" s="57"/>
       <c r="E5" s="4" t="s">
         <v>14</v>
       </c>
@@ -3575,12 +3569,12 @@
       </c>
     </row>
     <row r="6" spans="1:9" ht="69.95" customHeight="1">
-      <c r="A6" s="62"/>
+      <c r="A6" s="63"/>
       <c r="B6" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="C6" s="63"/>
-      <c r="D6" s="57"/>
+      <c r="C6" s="64"/>
+      <c r="D6" s="58"/>
       <c r="E6" s="4" t="s">
         <v>15</v>
       </c>
@@ -3590,7 +3584,7 @@
       <c r="I6" s="8"/>
     </row>
     <row r="7" spans="1:9">
-      <c r="A7" s="63"/>
+      <c r="A7" s="64"/>
       <c r="B7" s="9" t="s">
         <v>61</v>
       </c>
@@ -3674,41 +3668,41 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="23.25">
-      <c r="A1" s="60" t="s">
+      <c r="A1" s="61" t="s">
         <v>50</v>
       </c>
-      <c r="B1" s="60"/>
-      <c r="C1" s="79" t="s">
+      <c r="B1" s="61"/>
+      <c r="C1" s="80" t="s">
         <v>101</v>
       </c>
-      <c r="D1" s="79"/>
-      <c r="E1" s="79"/>
-      <c r="F1" s="79"/>
-      <c r="G1" s="79"/>
-      <c r="H1" s="79"/>
+      <c r="D1" s="80"/>
+      <c r="E1" s="80"/>
+      <c r="F1" s="80"/>
+      <c r="G1" s="80"/>
+      <c r="H1" s="80"/>
     </row>
     <row r="2" spans="1:11" ht="38.25" customHeight="1">
-      <c r="A2" s="84" t="s">
+      <c r="A2" s="85" t="s">
         <v>53</v>
       </c>
-      <c r="B2" s="84"/>
-      <c r="C2" s="80" t="s">
+      <c r="B2" s="85"/>
+      <c r="C2" s="81" t="s">
         <v>102</v>
       </c>
-      <c r="D2" s="80"/>
-      <c r="E2" s="80"/>
-      <c r="F2" s="80"/>
-      <c r="G2" s="80"/>
-      <c r="H2" s="80"/>
+      <c r="D2" s="81"/>
+      <c r="E2" s="81"/>
+      <c r="F2" s="81"/>
+      <c r="G2" s="81"/>
+      <c r="H2" s="81"/>
     </row>
     <row r="3" spans="1:11">
       <c r="A3" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="81" t="s">
+      <c r="B3" s="82" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="82"/>
+      <c r="C3" s="83"/>
       <c r="D3" s="13" t="s">
         <v>111</v>
       </c>
@@ -3735,14 +3729,14 @@
       </c>
     </row>
     <row r="4" spans="1:11" ht="15" customHeight="1">
-      <c r="A4" s="61" t="s">
+      <c r="A4" s="62" t="s">
         <v>57</v>
       </c>
-      <c r="B4" s="73" t="s">
+      <c r="B4" s="74" t="s">
         <v>104</v>
       </c>
-      <c r="C4" s="74"/>
-      <c r="D4" s="75"/>
+      <c r="C4" s="75"/>
+      <c r="D4" s="76"/>
       <c r="E4" s="30" t="s">
         <v>103</v>
       </c>
@@ -3766,11 +3760,11 @@
       </c>
     </row>
     <row r="5" spans="1:11" ht="51.75" customHeight="1">
-      <c r="A5" s="62"/>
-      <c r="B5" s="83" t="s">
+      <c r="A5" s="63"/>
+      <c r="B5" s="84" t="s">
         <v>107</v>
       </c>
-      <c r="C5" s="83"/>
+      <c r="C5" s="84"/>
       <c r="D5" s="34" t="s">
         <v>113</v>
       </c>
@@ -3797,12 +3791,12 @@
       </c>
     </row>
     <row r="6" spans="1:11" ht="33.75" customHeight="1">
-      <c r="A6" s="62"/>
-      <c r="B6" s="76" t="s">
+      <c r="A6" s="63"/>
+      <c r="B6" s="77" t="s">
         <v>112</v>
       </c>
-      <c r="C6" s="77"/>
-      <c r="D6" s="78"/>
+      <c r="C6" s="78"/>
+      <c r="D6" s="79"/>
       <c r="E6" s="30" t="s">
         <v>109</v>
       </c>
@@ -3826,11 +3820,11 @@
       </c>
     </row>
     <row r="7" spans="1:11" ht="31.5">
-      <c r="A7" s="62"/>
-      <c r="B7" s="67" t="s">
+      <c r="A7" s="63"/>
+      <c r="B7" s="68" t="s">
         <v>110</v>
       </c>
-      <c r="C7" s="68"/>
+      <c r="C7" s="69"/>
       <c r="D7" s="34" t="s">
         <v>114</v>
       </c>
@@ -3857,9 +3851,9 @@
       </c>
     </row>
     <row r="8" spans="1:11" ht="30">
-      <c r="A8" s="62"/>
-      <c r="B8" s="69"/>
-      <c r="C8" s="70"/>
+      <c r="A8" s="63"/>
+      <c r="B8" s="70"/>
+      <c r="C8" s="71"/>
       <c r="D8" s="35" t="s">
         <v>120</v>
       </c>
@@ -3886,9 +3880,9 @@
       </c>
     </row>
     <row r="9" spans="1:11" ht="31.5">
-      <c r="A9" s="62"/>
-      <c r="B9" s="69"/>
-      <c r="C9" s="70"/>
+      <c r="A9" s="63"/>
+      <c r="B9" s="70"/>
+      <c r="C9" s="71"/>
       <c r="D9" s="34" t="s">
         <v>121</v>
       </c>
@@ -3915,9 +3909,9 @@
       </c>
     </row>
     <row r="10" spans="1:11" ht="31.5">
-      <c r="A10" s="63"/>
-      <c r="B10" s="71"/>
-      <c r="C10" s="72"/>
+      <c r="A10" s="64"/>
+      <c r="B10" s="72"/>
+      <c r="C10" s="73"/>
       <c r="D10" s="34" t="s">
         <v>122</v>
       </c>
@@ -3983,11 +3977,11 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:8">
-      <c r="F3" s="87" t="s">
+      <c r="F3" s="88" t="s">
         <v>40</v>
       </c>
-      <c r="G3" s="88"/>
-      <c r="H3" s="88"/>
+      <c r="G3" s="89"/>
+      <c r="H3" s="89"/>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" s="6" t="s">
@@ -4016,7 +4010,7 @@
       </c>
     </row>
     <row r="5" spans="1:8">
-      <c r="A5" s="85" t="s">
+      <c r="A5" s="86" t="s">
         <v>28</v>
       </c>
       <c r="B5" s="23" t="s">
@@ -4042,7 +4036,7 @@
       </c>
     </row>
     <row r="6" spans="1:8">
-      <c r="A6" s="85"/>
+      <c r="A6" s="86"/>
       <c r="B6" s="23" t="s">
         <v>151</v>
       </c>
@@ -4066,7 +4060,7 @@
       </c>
     </row>
     <row r="7" spans="1:8">
-      <c r="A7" s="85"/>
+      <c r="A7" s="86"/>
       <c r="B7" s="23" t="s">
         <v>25</v>
       </c>
@@ -4090,7 +4084,7 @@
       </c>
     </row>
     <row r="8" spans="1:8">
-      <c r="A8" s="85"/>
+      <c r="A8" s="86"/>
       <c r="B8" s="23" t="s">
         <v>27</v>
       </c>
@@ -4114,7 +4108,7 @@
       </c>
     </row>
     <row r="9" spans="1:8" ht="30">
-      <c r="A9" s="86" t="s">
+      <c r="A9" s="87" t="s">
         <v>152</v>
       </c>
       <c r="B9" s="23" t="s">
@@ -4136,7 +4130,7 @@
       <c r="H9" s="41"/>
     </row>
     <row r="10" spans="1:8">
-      <c r="A10" s="86"/>
+      <c r="A10" s="87"/>
       <c r="B10" s="23" t="s">
         <v>153</v>
       </c>
@@ -4156,7 +4150,7 @@
       <c r="H10" s="41"/>
     </row>
     <row r="11" spans="1:8">
-      <c r="A11" s="86"/>
+      <c r="A11" s="87"/>
       <c r="B11" s="23" t="s">
         <v>154</v>
       </c>
@@ -4176,7 +4170,7 @@
       <c r="H11" s="41"/>
     </row>
     <row r="12" spans="1:8">
-      <c r="A12" s="86"/>
+      <c r="A12" s="87"/>
       <c r="B12" s="23" t="s">
         <v>155</v>
       </c>
@@ -4196,7 +4190,7 @@
       <c r="H12" s="41"/>
     </row>
     <row r="13" spans="1:8">
-      <c r="A13" s="86"/>
+      <c r="A13" s="87"/>
       <c r="B13" s="24" t="s">
         <v>156</v>
       </c>
@@ -4249,31 +4243,31 @@
       <c r="B1" s="37" t="s">
         <v>146</v>
       </c>
-      <c r="C1" s="89" t="s">
+      <c r="C1" s="90" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="90"/>
-      <c r="E1" s="91"/>
-      <c r="F1" s="89" t="s">
+      <c r="D1" s="91"/>
+      <c r="E1" s="92"/>
+      <c r="F1" s="90" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="90"/>
-      <c r="H1" s="91"/>
-      <c r="I1" s="89" t="s">
+      <c r="G1" s="91"/>
+      <c r="H1" s="92"/>
+      <c r="I1" s="90" t="s">
         <v>65</v>
       </c>
-      <c r="J1" s="90"/>
-      <c r="K1" s="91"/>
-      <c r="L1" s="92" t="s">
+      <c r="J1" s="91"/>
+      <c r="K1" s="92"/>
+      <c r="L1" s="93" t="s">
         <v>66</v>
       </c>
-      <c r="M1" s="93"/>
-      <c r="N1" s="93"/>
-      <c r="O1" s="89" t="s">
+      <c r="M1" s="94"/>
+      <c r="N1" s="94"/>
+      <c r="O1" s="90" t="s">
         <v>131</v>
       </c>
-      <c r="P1" s="90"/>
-      <c r="Q1" s="91"/>
+      <c r="P1" s="91"/>
+      <c r="Q1" s="92"/>
     </row>
     <row r="2" spans="1:17">
       <c r="A2" s="4" t="s">
@@ -4594,26 +4588,26 @@
       <c r="B1" s="37" t="s">
         <v>146</v>
       </c>
-      <c r="C1" s="89" t="s">
+      <c r="C1" s="90" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="90"/>
-      <c r="E1" s="91"/>
-      <c r="F1" s="89" t="s">
+      <c r="D1" s="91"/>
+      <c r="E1" s="92"/>
+      <c r="F1" s="90" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="90"/>
-      <c r="H1" s="91"/>
-      <c r="I1" s="89" t="s">
+      <c r="G1" s="91"/>
+      <c r="H1" s="92"/>
+      <c r="I1" s="90" t="s">
         <v>65</v>
       </c>
-      <c r="J1" s="90"/>
-      <c r="K1" s="91"/>
-      <c r="L1" s="92" t="s">
+      <c r="J1" s="91"/>
+      <c r="K1" s="92"/>
+      <c r="L1" s="93" t="s">
         <v>66</v>
       </c>
-      <c r="M1" s="93"/>
-      <c r="N1" s="93"/>
+      <c r="M1" s="94"/>
+      <c r="N1" s="94"/>
     </row>
     <row r="2" spans="1:14">
       <c r="A2" s="4" t="s">

</xml_diff>

<commit_message>
use script scope in pester
</commit_message>
<xml_diff>
--- a/JavaExcelBDD/src/test/resources/ExcelBDD.xlsx
+++ b/JavaExcelBDD/src/test/resources/ExcelBDD.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/2fe8b90741a02718/Git/SimpleOpenExcelBDD/JavaExcelBDD/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="75" documentId="13_ncr:1_{2BC08F18-7250-451B-B716-B852607D4077}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8ACF6F6D-D3E8-4B86-A32B-E9B921EE0738}"/>
+  <xr:revisionPtr revIDLastSave="81" documentId="13_ncr:1_{2BC08F18-7250-451B-B716-B852607D4077}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BDD96103-1865-41AC-AC4F-6F41B3C4A984}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="6" xr2:uid="{965C72BA-AC7B-4020-96A1-B4855C2F0853}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="5" xr2:uid="{965C72BA-AC7B-4020-96A1-B4855C2F0853}"/>
   </bookViews>
   <sheets>
     <sheet name="SimpleOpenBDD" sheetId="1" r:id="rId1"/>
@@ -620,19 +620,19 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -871,7 +871,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="96">
+  <cellXfs count="97">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -940,10 +940,10 @@
     <xf numFmtId="9" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1034,22 +1034,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1061,17 +1061,14 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -1082,11 +1079,8 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -1117,6 +1111,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -2095,36 +2098,36 @@
       <c r="D1" s="37" t="s">
         <v>146</v>
       </c>
-      <c r="E1" s="90" t="s">
+      <c r="E1" s="88" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="91"/>
-      <c r="G1" s="92"/>
-      <c r="H1" s="90" t="s">
+      <c r="F1" s="89"/>
+      <c r="G1" s="90"/>
+      <c r="H1" s="88" t="s">
         <v>4</v>
       </c>
-      <c r="I1" s="91"/>
-      <c r="J1" s="92"/>
-      <c r="K1" s="90" t="s">
+      <c r="I1" s="89"/>
+      <c r="J1" s="90"/>
+      <c r="K1" s="88" t="s">
         <v>65</v>
       </c>
-      <c r="L1" s="91"/>
-      <c r="M1" s="92"/>
-      <c r="N1" s="95" t="s">
+      <c r="L1" s="89"/>
+      <c r="M1" s="90"/>
+      <c r="N1" s="93" t="s">
         <v>66</v>
       </c>
-      <c r="O1" s="95"/>
-      <c r="P1" s="95"/>
-      <c r="Q1" s="90" t="s">
+      <c r="O1" s="93"/>
+      <c r="P1" s="93"/>
+      <c r="Q1" s="88" t="s">
         <v>131</v>
       </c>
-      <c r="R1" s="91"/>
-      <c r="S1" s="92"/>
-      <c r="T1" s="90" t="s">
+      <c r="R1" s="89"/>
+      <c r="S1" s="90"/>
+      <c r="T1" s="88" t="s">
         <v>163</v>
       </c>
-      <c r="U1" s="91"/>
-      <c r="V1" s="92"/>
+      <c r="U1" s="89"/>
+      <c r="V1" s="90"/>
     </row>
     <row r="2" spans="1:22">
       <c r="A2" s="4" t="s">
@@ -2514,31 +2517,31 @@
       <c r="D3" s="37" t="s">
         <v>146</v>
       </c>
-      <c r="E3" s="90" t="s">
+      <c r="E3" s="88" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="91"/>
-      <c r="G3" s="92"/>
-      <c r="H3" s="90" t="s">
+      <c r="F3" s="89"/>
+      <c r="G3" s="90"/>
+      <c r="H3" s="88" t="s">
         <v>4</v>
       </c>
-      <c r="I3" s="91"/>
-      <c r="J3" s="92"/>
-      <c r="K3" s="90" t="s">
+      <c r="I3" s="89"/>
+      <c r="J3" s="90"/>
+      <c r="K3" s="88" t="s">
         <v>65</v>
       </c>
-      <c r="L3" s="91"/>
-      <c r="M3" s="92"/>
-      <c r="N3" s="95" t="s">
+      <c r="L3" s="89"/>
+      <c r="M3" s="90"/>
+      <c r="N3" s="93" t="s">
         <v>66</v>
       </c>
-      <c r="O3" s="95"/>
-      <c r="P3" s="95"/>
-      <c r="Q3" s="90" t="s">
+      <c r="O3" s="93"/>
+      <c r="P3" s="93"/>
+      <c r="Q3" s="88" t="s">
         <v>131</v>
       </c>
-      <c r="R3" s="91"/>
-      <c r="S3" s="92"/>
+      <c r="R3" s="89"/>
+      <c r="S3" s="90"/>
     </row>
     <row r="4" spans="1:19">
       <c r="A4" s="4" t="s">
@@ -3663,8 +3666,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5B5B253-4765-4799-B65C-A6D3EFCA81AD}">
   <dimension ref="A1:K10"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3679,42 +3682,42 @@
     <col min="8" max="8" width="9.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="23.25">
-      <c r="A1" s="61" t="s">
+    <row r="1" spans="1:11" ht="21">
+      <c r="A1" s="94" t="s">
         <v>50</v>
       </c>
-      <c r="B1" s="61"/>
-      <c r="C1" s="80" t="s">
+      <c r="B1" s="94"/>
+      <c r="C1" s="96" t="s">
         <v>101</v>
       </c>
-      <c r="D1" s="80"/>
-      <c r="E1" s="80"/>
-      <c r="F1" s="80"/>
-      <c r="G1" s="80"/>
-      <c r="H1" s="80"/>
+      <c r="D1" s="96"/>
+      <c r="E1" s="96"/>
+      <c r="F1" s="96"/>
+      <c r="G1" s="96"/>
+      <c r="H1" s="96"/>
     </row>
     <row r="2" spans="1:11" ht="38.25" customHeight="1">
-      <c r="A2" s="85" t="s">
+      <c r="A2" s="95" t="s">
         <v>53</v>
       </c>
-      <c r="B2" s="85"/>
-      <c r="C2" s="81" t="s">
+      <c r="B2" s="95"/>
+      <c r="C2" s="80" t="s">
         <v>102</v>
       </c>
-      <c r="D2" s="81"/>
-      <c r="E2" s="81"/>
-      <c r="F2" s="81"/>
-      <c r="G2" s="81"/>
-      <c r="H2" s="81"/>
+      <c r="D2" s="80"/>
+      <c r="E2" s="80"/>
+      <c r="F2" s="80"/>
+      <c r="G2" s="80"/>
+      <c r="H2" s="80"/>
     </row>
     <row r="3" spans="1:11">
       <c r="A3" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="82" t="s">
+      <c r="B3" s="81" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="83"/>
+      <c r="C3" s="82"/>
       <c r="D3" s="13" t="s">
         <v>111</v>
       </c>
@@ -3773,10 +3776,10 @@
     </row>
     <row r="5" spans="1:11" ht="51.75" customHeight="1">
       <c r="A5" s="63"/>
-      <c r="B5" s="84" t="s">
+      <c r="B5" s="83" t="s">
         <v>107</v>
       </c>
-      <c r="C5" s="84"/>
+      <c r="C5" s="83"/>
       <c r="D5" s="34" t="s">
         <v>113</v>
       </c>
@@ -3972,7 +3975,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACCEE44C-3384-41FF-9A79-FA3C44CB5ED1}">
   <dimension ref="A3:H17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
@@ -3989,11 +3992,11 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:8">
-      <c r="F3" s="88" t="s">
+      <c r="F3" s="86" t="s">
         <v>40</v>
       </c>
-      <c r="G3" s="89"/>
-      <c r="H3" s="89"/>
+      <c r="G3" s="87"/>
+      <c r="H3" s="87"/>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" s="6" t="s">
@@ -4022,7 +4025,7 @@
       </c>
     </row>
     <row r="5" spans="1:8">
-      <c r="A5" s="86" t="s">
+      <c r="A5" s="84" t="s">
         <v>28</v>
       </c>
       <c r="B5" s="23" t="s">
@@ -4048,7 +4051,7 @@
       </c>
     </row>
     <row r="6" spans="1:8">
-      <c r="A6" s="86"/>
+      <c r="A6" s="84"/>
       <c r="B6" s="23" t="s">
         <v>151</v>
       </c>
@@ -4072,7 +4075,7 @@
       </c>
     </row>
     <row r="7" spans="1:8">
-      <c r="A7" s="86"/>
+      <c r="A7" s="84"/>
       <c r="B7" s="23" t="s">
         <v>25</v>
       </c>
@@ -4096,7 +4099,7 @@
       </c>
     </row>
     <row r="8" spans="1:8">
-      <c r="A8" s="86"/>
+      <c r="A8" s="84"/>
       <c r="B8" s="23" t="s">
         <v>27</v>
       </c>
@@ -4120,7 +4123,7 @@
       </c>
     </row>
     <row r="9" spans="1:8" ht="30">
-      <c r="A9" s="87" t="s">
+      <c r="A9" s="85" t="s">
         <v>172</v>
       </c>
       <c r="B9" s="23" t="s">
@@ -4141,7 +4144,7 @@
       <c r="H9" s="41"/>
     </row>
     <row r="10" spans="1:8">
-      <c r="A10" s="87"/>
+      <c r="A10" s="85"/>
       <c r="B10" s="23" t="s">
         <v>152</v>
       </c>
@@ -4163,7 +4166,7 @@
       <c r="H10" s="41"/>
     </row>
     <row r="11" spans="1:8">
-      <c r="A11" s="87"/>
+      <c r="A11" s="85"/>
       <c r="B11" s="23" t="s">
         <v>153</v>
       </c>
@@ -4183,7 +4186,7 @@
       <c r="H11" s="41"/>
     </row>
     <row r="12" spans="1:8">
-      <c r="A12" s="87"/>
+      <c r="A12" s="85"/>
       <c r="B12" s="23" t="s">
         <v>154</v>
       </c>
@@ -4203,7 +4206,7 @@
       <c r="H12" s="41"/>
     </row>
     <row r="13" spans="1:8">
-      <c r="A13" s="87"/>
+      <c r="A13" s="85"/>
       <c r="B13" s="24" t="s">
         <v>155</v>
       </c>
@@ -4312,31 +4315,31 @@
       <c r="B1" s="37" t="s">
         <v>146</v>
       </c>
-      <c r="C1" s="90" t="s">
+      <c r="C1" s="88" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="91"/>
-      <c r="E1" s="92"/>
-      <c r="F1" s="90" t="s">
+      <c r="D1" s="89"/>
+      <c r="E1" s="90"/>
+      <c r="F1" s="88" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="91"/>
-      <c r="H1" s="92"/>
-      <c r="I1" s="90" t="s">
+      <c r="G1" s="89"/>
+      <c r="H1" s="90"/>
+      <c r="I1" s="88" t="s">
         <v>65</v>
       </c>
-      <c r="J1" s="91"/>
-      <c r="K1" s="92"/>
-      <c r="L1" s="93" t="s">
+      <c r="J1" s="89"/>
+      <c r="K1" s="90"/>
+      <c r="L1" s="91" t="s">
         <v>66</v>
       </c>
-      <c r="M1" s="94"/>
-      <c r="N1" s="94"/>
-      <c r="O1" s="90" t="s">
+      <c r="M1" s="92"/>
+      <c r="N1" s="92"/>
+      <c r="O1" s="88" t="s">
         <v>131</v>
       </c>
-      <c r="P1" s="91"/>
-      <c r="Q1" s="92"/>
+      <c r="P1" s="89"/>
+      <c r="Q1" s="90"/>
     </row>
     <row r="2" spans="1:17">
       <c r="A2" s="4" t="s">
@@ -4657,26 +4660,26 @@
       <c r="B1" s="37" t="s">
         <v>146</v>
       </c>
-      <c r="C1" s="90" t="s">
+      <c r="C1" s="88" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="91"/>
-      <c r="E1" s="92"/>
-      <c r="F1" s="90" t="s">
+      <c r="D1" s="89"/>
+      <c r="E1" s="90"/>
+      <c r="F1" s="88" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="91"/>
-      <c r="H1" s="92"/>
-      <c r="I1" s="90" t="s">
+      <c r="G1" s="89"/>
+      <c r="H1" s="90"/>
+      <c r="I1" s="88" t="s">
         <v>65</v>
       </c>
-      <c r="J1" s="91"/>
-      <c r="K1" s="92"/>
-      <c r="L1" s="93" t="s">
+      <c r="J1" s="89"/>
+      <c r="K1" s="90"/>
+      <c r="L1" s="91" t="s">
         <v>66</v>
       </c>
-      <c r="M1" s="94"/>
-      <c r="N1" s="94"/>
+      <c r="M1" s="92"/>
+      <c r="N1" s="92"/>
     </row>
     <row r="2" spans="1:14">
       <c r="A2" s="4" t="s">

</xml_diff>